<commit_message>
Modifica largos pisos, corrige formato
</commit_message>
<xml_diff>
--- a/Tarea 02/Largos-muros.xlsx
+++ b/Tarea 02/Largos-muros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Google Drive\Trabajos\Proyecto de Hormigón Armado\proyecto-CI5206\Tarea 02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{84D2E54C-84E0-4D18-8F6D-C2A6B4C58146}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0C877A02-F512-4A82-BED8-370E12ED8C98}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{02DCFF44-6514-457A-8521-53C0490CA4AF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>N° piso</t>
   </si>
@@ -166,14 +166,21 @@
   </si>
   <si>
     <t>torre + medio est</t>
+  </si>
+  <si>
+    <t>% TauX</t>
+  </si>
+  <si>
+    <t>% TauY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -199,18 +206,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -220,13 +221,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -236,46 +231,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="23">
+  <borders count="20">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -389,13 +351,26 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -407,70 +382,14 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -517,6 +436,17 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -548,7 +478,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -563,169 +493,151 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1054,10 +966,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86364C21-7A4B-487E-B815-3438660120DA}">
-  <dimension ref="A1:AD28"/>
+  <dimension ref="A1:AF28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="P1" sqref="M1:P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1072,13 +984,13 @@
     <col min="11" max="11" width="5.33203125" customWidth="1"/>
     <col min="12" max="12" width="7.5546875" customWidth="1"/>
     <col min="13" max="13" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.44140625" customWidth="1"/>
-    <col min="16" max="16" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="21" max="29" width="11.5546875" style="1"/>
+    <col min="14" max="16" width="8.44140625" customWidth="1"/>
+    <col min="18" max="18" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="23" max="31" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
@@ -1088,76 +1000,82 @@
       <c r="D2" s="1">
         <v>410.4</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="9" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="19" t="s">
+      <c r="M2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="20" t="s">
+      <c r="N2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="20" t="s">
+      <c r="O2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="37" t="s">
+      <c r="S2" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="38" t="s">
+      <c r="T2" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="U2" s="19" t="s">
+      <c r="W2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="V2" s="20" t="s">
+      <c r="X2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="W2" s="19" t="s">
+      <c r="Y2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="X2" s="20" t="s">
+      <c r="Z2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="Y2" s="19" t="s">
+      <c r="AA2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="Z2" s="20" t="s">
+      <c r="AB2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="19" t="s">
+      <c r="AC2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="20" t="s">
+      <c r="AD2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="AC2" s="19" t="str">
+      <c r="AE2" s="8" t="str">
         <f>"-1 Y"</f>
         <v>-1 Y</v>
       </c>
-      <c r="AD2" s="20" t="str">
+      <c r="AF2" s="9" t="str">
         <f>"-1 X"</f>
         <v>-1 X</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1168,71 +1086,79 @@
         <v>1</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="15">
+      <c r="F3" s="52">
         <v>23</v>
       </c>
-      <c r="G3" s="21">
+      <c r="G3" s="49">
         <f>$D$2*$D$4*$D$5</f>
         <v>41.04</v>
       </c>
-      <c r="H3" s="22">
+      <c r="H3" s="53">
         <f>G3</f>
         <v>41.04</v>
       </c>
-      <c r="I3" s="32">
-        <f>$V$25</f>
+      <c r="I3" s="18">
+        <f>$X$25</f>
         <v>61.86</v>
       </c>
-      <c r="J3" s="33">
-        <f>$U$25</f>
+      <c r="J3" s="14">
+        <f>$W$25</f>
         <v>53.12</v>
       </c>
-      <c r="K3" s="61">
-        <v>0.2</v>
-      </c>
-      <c r="L3" s="62">
-        <v>0.2</v>
-      </c>
-      <c r="M3" s="32">
+      <c r="K3" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="L3" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="M3" s="13">
         <f t="shared" ref="M3:M22" si="0">I3*K3*$D$8*100*100</f>
         <v>866.04</v>
       </c>
-      <c r="N3" s="33">
+      <c r="N3" s="18">
         <f>J3*L3*$D$8*100*100</f>
         <v>743.68000000000006</v>
       </c>
-      <c r="O3" s="24" t="str">
+      <c r="O3" s="38">
+        <f>H3/M3</f>
+        <v>4.738811140363032E-2</v>
+      </c>
+      <c r="P3" s="40">
+        <f>H3/N3</f>
+        <v>5.5185025817555931E-2</v>
+      </c>
+      <c r="Q3" s="11" t="str">
         <f>IF(OR(M3&lt;H3,N3&lt;H3),"MALO","WENO")</f>
         <v>WENO</v>
       </c>
-      <c r="Q3" s="39">
+      <c r="S3" s="23">
         <f>M3-H3</f>
         <v>825</v>
       </c>
-      <c r="R3" s="40">
+      <c r="T3" s="24">
         <f>N3-H3</f>
         <v>702.6400000000001</v>
       </c>
-      <c r="U3" s="23">
+      <c r="W3" s="10">
         <v>3.17</v>
       </c>
-      <c r="V3" s="24">
+      <c r="X3" s="11">
         <v>1.6</v>
       </c>
-      <c r="W3" s="23">
+      <c r="Y3" s="10">
         <v>2.5099999999999998</v>
       </c>
-      <c r="X3" s="24">
+      <c r="Z3" s="11">
         <v>1.9</v>
       </c>
-      <c r="Y3" s="23"/>
-      <c r="Z3" s="24"/>
-      <c r="AA3" s="23"/>
-      <c r="AB3" s="24"/>
-      <c r="AC3" s="23"/>
-      <c r="AD3" s="24"/>
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="11"/>
+      <c r="AC3" s="10"/>
+      <c r="AD3" s="11"/>
+      <c r="AE3" s="10"/>
+      <c r="AF3" s="11"/>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1243,69 +1169,77 @@
         <v>1</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="10">
+      <c r="F4" s="52">
         <v>22</v>
       </c>
-      <c r="G4" s="6">
-        <f t="shared" ref="G4:G26" si="1">$D$2*$D$4*$D$5</f>
+      <c r="G4" s="49">
+        <f t="shared" ref="G4:G24" si="1">$D$2*$D$4*$D$5</f>
         <v>41.04</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="53">
         <f>H3+G4</f>
         <v>82.08</v>
       </c>
-      <c r="I4" s="32">
-        <f t="shared" ref="I4:I22" si="2">$V$25</f>
+      <c r="I4" s="18">
+        <f t="shared" ref="I4:I22" si="2">$X$25</f>
         <v>61.86</v>
       </c>
-      <c r="J4" s="33">
-        <f t="shared" ref="J4:J22" si="3">$U$25</f>
+      <c r="J4" s="14">
+        <f t="shared" ref="J4:J22" si="3">$W$25</f>
         <v>53.12</v>
       </c>
-      <c r="K4" s="61">
-        <v>0.2</v>
-      </c>
-      <c r="L4" s="62">
-        <v>0.2</v>
-      </c>
-      <c r="M4" s="32">
+      <c r="K4" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="L4" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="M4" s="13">
         <f t="shared" si="0"/>
         <v>866.04</v>
       </c>
-      <c r="N4" s="33">
+      <c r="N4" s="18">
         <f t="shared" ref="N4:N22" si="4">J4*L4*$D$8*100*100</f>
         <v>743.68000000000006</v>
       </c>
-      <c r="O4" s="24" t="str">
-        <f t="shared" ref="O4:O26" si="5">IF(OR(M4&lt;H4,N4&lt;H4),"MALO","WENO")</f>
+      <c r="O4" s="38">
+        <f t="shared" ref="O4:O26" si="5">H4/M4</f>
+        <v>9.4776222807260641E-2</v>
+      </c>
+      <c r="P4" s="40">
+        <f t="shared" ref="P4:P26" si="6">H4/N4</f>
+        <v>0.11037005163511186</v>
+      </c>
+      <c r="Q4" s="11" t="str">
+        <f t="shared" ref="Q4:Q26" si="7">IF(OR(M4&lt;H4,N4&lt;H4),"MALO","WENO")</f>
         <v>WENO</v>
       </c>
-      <c r="Q4" s="41">
-        <f t="shared" ref="Q4:Q26" si="6">M4-H4</f>
+      <c r="S4" s="25">
+        <f t="shared" ref="S4:S26" si="8">M4-H4</f>
         <v>783.95999999999992</v>
       </c>
-      <c r="R4" s="42">
-        <f t="shared" ref="R4:R26" si="7">N4-H4</f>
+      <c r="T4" s="26">
+        <f t="shared" ref="T4:T26" si="9">N4-H4</f>
         <v>661.6</v>
       </c>
-      <c r="U4" s="23"/>
-      <c r="V4" s="24">
+      <c r="W4" s="10"/>
+      <c r="X4" s="11">
         <v>1.9</v>
       </c>
-      <c r="W4" s="23">
+      <c r="Y4" s="10">
         <v>5.3369999999999997</v>
       </c>
-      <c r="X4" s="24">
+      <c r="Z4" s="11">
         <v>1.6</v>
       </c>
-      <c r="Y4" s="23"/>
-      <c r="Z4" s="24"/>
-      <c r="AA4" s="23"/>
-      <c r="AB4" s="24"/>
-      <c r="AC4" s="23"/>
-      <c r="AD4" s="24"/>
+      <c r="AA4" s="10"/>
+      <c r="AB4" s="11"/>
+      <c r="AC4" s="10"/>
+      <c r="AD4" s="11"/>
+      <c r="AE4" s="10"/>
+      <c r="AF4" s="11"/>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1316,67 +1250,75 @@
         <v>0.1</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="10">
+      <c r="F5" s="52">
         <v>21</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H5" s="25">
-        <f t="shared" ref="H5:H26" si="8">H4+G5</f>
+      <c r="H5" s="53">
+        <f t="shared" ref="H5:H26" si="10">H4+G5</f>
         <v>123.12</v>
       </c>
-      <c r="I5" s="32">
+      <c r="I5" s="18">
         <f t="shared" si="2"/>
         <v>61.86</v>
       </c>
-      <c r="J5" s="33">
+      <c r="J5" s="14">
         <f t="shared" si="3"/>
         <v>53.12</v>
       </c>
-      <c r="K5" s="61">
-        <v>0.2</v>
-      </c>
-      <c r="L5" s="62">
-        <v>0.2</v>
-      </c>
-      <c r="M5" s="32">
+      <c r="K5" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="L5" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="M5" s="13">
         <f t="shared" si="0"/>
         <v>866.04</v>
       </c>
-      <c r="N5" s="33">
+      <c r="N5" s="18">
         <f t="shared" si="4"/>
         <v>743.68000000000006</v>
       </c>
-      <c r="O5" s="24" t="str">
+      <c r="O5" s="38">
         <f t="shared" si="5"/>
+        <v>0.14216433421089097</v>
+      </c>
+      <c r="P5" s="40">
+        <f t="shared" si="6"/>
+        <v>0.16555507745266781</v>
+      </c>
+      <c r="Q5" s="11" t="str">
+        <f t="shared" si="7"/>
         <v>WENO</v>
       </c>
-      <c r="Q5" s="41">
-        <f t="shared" si="6"/>
+      <c r="S5" s="25">
+        <f t="shared" si="8"/>
         <v>742.92</v>
       </c>
-      <c r="R5" s="42">
-        <f t="shared" si="7"/>
+      <c r="T5" s="26">
+        <f t="shared" si="9"/>
         <v>620.56000000000006</v>
       </c>
-      <c r="U5" s="23"/>
-      <c r="V5" s="24"/>
-      <c r="W5" s="23">
+      <c r="W5" s="10"/>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="10">
         <v>3.17</v>
       </c>
-      <c r="X5" s="24">
+      <c r="Z5" s="11">
         <v>3.39</v>
       </c>
-      <c r="Y5" s="23"/>
-      <c r="Z5" s="24"/>
-      <c r="AA5" s="23"/>
-      <c r="AB5" s="24"/>
-      <c r="AC5" s="23"/>
-      <c r="AD5" s="24"/>
+      <c r="AA5" s="10"/>
+      <c r="AB5" s="11"/>
+      <c r="AC5" s="10"/>
+      <c r="AD5" s="11"/>
+      <c r="AE5" s="10"/>
+      <c r="AF5" s="11"/>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
@@ -1387,138 +1329,154 @@
         <v>7</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="10">
+      <c r="F6" s="52">
         <v>20</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H6" s="25">
-        <f t="shared" si="8"/>
+      <c r="H6" s="53">
+        <f t="shared" si="10"/>
         <v>164.16</v>
       </c>
-      <c r="I6" s="32">
+      <c r="I6" s="18">
         <f t="shared" si="2"/>
         <v>61.86</v>
       </c>
-      <c r="J6" s="33">
+      <c r="J6" s="14">
         <f t="shared" si="3"/>
         <v>53.12</v>
       </c>
-      <c r="K6" s="61">
-        <v>0.2</v>
-      </c>
-      <c r="L6" s="62">
-        <v>0.2</v>
-      </c>
-      <c r="M6" s="32">
+      <c r="K6" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="L6" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="M6" s="13">
         <f t="shared" si="0"/>
         <v>866.04</v>
       </c>
-      <c r="N6" s="33">
+      <c r="N6" s="18">
         <f t="shared" si="4"/>
         <v>743.68000000000006</v>
       </c>
-      <c r="O6" s="24" t="str">
+      <c r="O6" s="38">
         <f t="shared" si="5"/>
+        <v>0.18955244561452128</v>
+      </c>
+      <c r="P6" s="40">
+        <f t="shared" si="6"/>
+        <v>0.22074010327022373</v>
+      </c>
+      <c r="Q6" s="11" t="str">
+        <f t="shared" si="7"/>
         <v>WENO</v>
       </c>
-      <c r="Q6" s="41">
-        <f t="shared" si="6"/>
+      <c r="S6" s="25">
+        <f t="shared" si="8"/>
         <v>701.88</v>
       </c>
-      <c r="R6" s="42">
-        <f t="shared" si="7"/>
+      <c r="T6" s="26">
+        <f t="shared" si="9"/>
         <v>579.5200000000001</v>
       </c>
-      <c r="U6" s="23">
+      <c r="W6" s="10">
         <v>3.17</v>
       </c>
-      <c r="V6" s="24">
+      <c r="X6" s="11">
         <v>3.39</v>
       </c>
-      <c r="W6" s="23">
+      <c r="Y6" s="10">
         <v>4.5999999999999996</v>
       </c>
-      <c r="X6" s="24">
+      <c r="Z6" s="11">
         <v>1.6</v>
       </c>
-      <c r="Y6" s="23"/>
-      <c r="Z6" s="24"/>
-      <c r="AA6" s="23"/>
-      <c r="AB6" s="24"/>
-      <c r="AC6" s="23"/>
-      <c r="AD6" s="24"/>
+      <c r="AA6" s="10"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="10"/>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="10"/>
+      <c r="AF6" s="11"/>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="F7" s="10">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="F7" s="52">
         <v>19</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H7" s="25">
-        <f t="shared" si="8"/>
+      <c r="H7" s="53">
+        <f t="shared" si="10"/>
         <v>205.2</v>
       </c>
-      <c r="I7" s="32">
+      <c r="I7" s="18">
         <f t="shared" si="2"/>
         <v>61.86</v>
       </c>
-      <c r="J7" s="33">
+      <c r="J7" s="14">
         <f t="shared" si="3"/>
         <v>53.12</v>
       </c>
-      <c r="K7" s="61">
-        <v>0.2</v>
-      </c>
-      <c r="L7" s="62">
-        <v>0.2</v>
-      </c>
-      <c r="M7" s="32">
+      <c r="K7" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="L7" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="M7" s="13">
         <f t="shared" si="0"/>
         <v>866.04</v>
       </c>
-      <c r="N7" s="33">
+      <c r="N7" s="18">
         <f t="shared" si="4"/>
         <v>743.68000000000006</v>
       </c>
-      <c r="O7" s="24" t="str">
+      <c r="O7" s="38">
         <f t="shared" si="5"/>
+        <v>0.23694055701815159</v>
+      </c>
+      <c r="P7" s="40">
+        <f t="shared" si="6"/>
+        <v>0.27592512908777966</v>
+      </c>
+      <c r="Q7" s="11" t="str">
+        <f t="shared" si="7"/>
         <v>WENO</v>
       </c>
-      <c r="Q7" s="41">
-        <f t="shared" si="6"/>
+      <c r="S7" s="25">
+        <f t="shared" si="8"/>
         <v>660.83999999999992</v>
       </c>
-      <c r="R7" s="42">
-        <f t="shared" si="7"/>
+      <c r="T7" s="26">
+        <f t="shared" si="9"/>
         <v>538.48</v>
       </c>
-      <c r="U7" s="23">
+      <c r="W7" s="10">
         <v>5.3369999999999997</v>
       </c>
-      <c r="V7" s="24">
+      <c r="X7" s="11">
         <v>1.6</v>
       </c>
-      <c r="W7" s="23">
+      <c r="Y7" s="10">
         <v>2</v>
       </c>
-      <c r="X7" s="24">
+      <c r="Z7" s="11">
         <v>1.92</v>
       </c>
-      <c r="Y7" s="23"/>
-      <c r="Z7" s="24"/>
-      <c r="AA7" s="23"/>
-      <c r="AB7" s="24"/>
-      <c r="AC7" s="23"/>
-      <c r="AD7" s="24"/>
+      <c r="AA7" s="10"/>
+      <c r="AB7" s="11"/>
+      <c r="AC7" s="10"/>
+      <c r="AD7" s="11"/>
+      <c r="AE7" s="10"/>
+      <c r="AF7" s="11"/>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="37" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1528,836 +1486,933 @@
         <f>D6/1000</f>
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="52">
         <v>18</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H8" s="25">
-        <f t="shared" si="8"/>
+      <c r="H8" s="53">
+        <f t="shared" si="10"/>
         <v>246.23999999999998</v>
       </c>
-      <c r="I8" s="32">
+      <c r="I8" s="18">
         <f t="shared" si="2"/>
         <v>61.86</v>
       </c>
-      <c r="J8" s="33">
+      <c r="J8" s="14">
         <f t="shared" si="3"/>
         <v>53.12</v>
       </c>
-      <c r="K8" s="61">
-        <v>0.2</v>
-      </c>
-      <c r="L8" s="62">
-        <v>0.2</v>
-      </c>
-      <c r="M8" s="32">
+      <c r="K8" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="L8" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="M8" s="13">
         <f t="shared" si="0"/>
         <v>866.04</v>
       </c>
-      <c r="N8" s="33">
+      <c r="N8" s="18">
         <f t="shared" si="4"/>
         <v>743.68000000000006</v>
       </c>
-      <c r="O8" s="24" t="str">
+      <c r="O8" s="38">
         <f t="shared" si="5"/>
+        <v>0.28432866842178189</v>
+      </c>
+      <c r="P8" s="40">
+        <f t="shared" si="6"/>
+        <v>0.33111015490533557</v>
+      </c>
+      <c r="Q8" s="11" t="str">
+        <f t="shared" si="7"/>
         <v>WENO</v>
       </c>
-      <c r="Q8" s="41">
-        <f t="shared" si="6"/>
+      <c r="S8" s="25">
+        <f t="shared" si="8"/>
         <v>619.79999999999995</v>
       </c>
-      <c r="R8" s="42">
-        <f t="shared" si="7"/>
+      <c r="T8" s="26">
+        <f t="shared" si="9"/>
         <v>497.44000000000005</v>
       </c>
-      <c r="U8" s="23">
+      <c r="W8" s="10">
         <v>4.5999999999999996</v>
       </c>
-      <c r="V8" s="24">
+      <c r="X8" s="11">
         <v>1.92</v>
       </c>
-      <c r="W8" s="23">
+      <c r="Y8" s="10">
         <v>5.46</v>
       </c>
-      <c r="X8" s="24">
+      <c r="Z8" s="11">
         <v>6.359</v>
       </c>
-      <c r="Y8" s="23"/>
-      <c r="Z8" s="24"/>
-      <c r="AA8" s="23"/>
-      <c r="AB8" s="24"/>
-      <c r="AC8" s="23"/>
-      <c r="AD8" s="24"/>
+      <c r="AA8" s="10"/>
+      <c r="AB8" s="11"/>
+      <c r="AC8" s="10"/>
+      <c r="AD8" s="11"/>
+      <c r="AE8" s="10"/>
+      <c r="AF8" s="11"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
-      <c r="B9" s="53"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="4"/>
       <c r="D9" s="5"/>
-      <c r="F9" s="10">
+      <c r="F9" s="52">
         <v>17</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H9" s="25">
-        <f t="shared" si="8"/>
+      <c r="H9" s="53">
+        <f t="shared" si="10"/>
         <v>287.27999999999997</v>
       </c>
-      <c r="I9" s="32">
+      <c r="I9" s="18">
         <f t="shared" si="2"/>
         <v>61.86</v>
       </c>
-      <c r="J9" s="33">
+      <c r="J9" s="14">
         <f t="shared" si="3"/>
         <v>53.12</v>
       </c>
-      <c r="K9" s="61">
-        <v>0.2</v>
-      </c>
-      <c r="L9" s="62">
-        <v>0.2</v>
-      </c>
-      <c r="M9" s="32">
+      <c r="K9" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="L9" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="M9" s="13">
         <f t="shared" si="0"/>
         <v>866.04</v>
       </c>
-      <c r="N9" s="33">
+      <c r="N9" s="18">
         <f t="shared" si="4"/>
         <v>743.68000000000006</v>
       </c>
-      <c r="O9" s="24" t="str">
+      <c r="O9" s="38">
         <f t="shared" si="5"/>
+        <v>0.3317167798254122</v>
+      </c>
+      <c r="P9" s="40">
+        <f t="shared" si="6"/>
+        <v>0.38629518072289148</v>
+      </c>
+      <c r="Q9" s="11" t="str">
+        <f t="shared" si="7"/>
         <v>WENO</v>
       </c>
-      <c r="Q9" s="41">
-        <f t="shared" si="6"/>
+      <c r="S9" s="25">
+        <f t="shared" si="8"/>
         <v>578.76</v>
       </c>
-      <c r="R9" s="42">
-        <f t="shared" si="7"/>
+      <c r="T9" s="26">
+        <f t="shared" si="9"/>
         <v>456.40000000000009</v>
       </c>
-      <c r="U9" s="23"/>
-      <c r="V9" s="24">
+      <c r="W9" s="10"/>
+      <c r="X9" s="11">
         <v>6.359</v>
       </c>
-      <c r="W9" s="23">
+      <c r="Y9" s="10">
         <v>4.05</v>
       </c>
-      <c r="X9" s="24">
+      <c r="Z9" s="11">
         <v>5.0330000000000004</v>
       </c>
-      <c r="Y9" s="23"/>
-      <c r="Z9" s="24"/>
-      <c r="AA9" s="23"/>
-      <c r="AB9" s="24"/>
-      <c r="AC9" s="23"/>
-      <c r="AD9" s="24"/>
+      <c r="AA9" s="10"/>
+      <c r="AB9" s="11"/>
+      <c r="AC9" s="10"/>
+      <c r="AD9" s="11"/>
+      <c r="AE9" s="10"/>
+      <c r="AF9" s="11"/>
     </row>
-    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
-      <c r="B10" s="53"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="4"/>
       <c r="D10" s="5"/>
-      <c r="F10" s="10">
+      <c r="F10" s="52">
         <v>16</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H10" s="25">
-        <f t="shared" si="8"/>
+      <c r="H10" s="53">
+        <f t="shared" si="10"/>
         <v>328.32</v>
       </c>
-      <c r="I10" s="32">
+      <c r="I10" s="18">
         <f t="shared" si="2"/>
         <v>61.86</v>
       </c>
-      <c r="J10" s="33">
+      <c r="J10" s="14">
         <f t="shared" si="3"/>
         <v>53.12</v>
       </c>
-      <c r="K10" s="61">
-        <v>0.2</v>
-      </c>
-      <c r="L10" s="62">
-        <v>0.2</v>
-      </c>
-      <c r="M10" s="32">
+      <c r="K10" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="L10" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="M10" s="13">
         <f t="shared" si="0"/>
         <v>866.04</v>
       </c>
-      <c r="N10" s="33">
+      <c r="N10" s="18">
         <f t="shared" si="4"/>
         <v>743.68000000000006</v>
       </c>
-      <c r="O10" s="24" t="str">
+      <c r="O10" s="38">
         <f t="shared" si="5"/>
+        <v>0.37910489122904256</v>
+      </c>
+      <c r="P10" s="40">
+        <f t="shared" si="6"/>
+        <v>0.44148020654044745</v>
+      </c>
+      <c r="Q10" s="11" t="str">
+        <f t="shared" si="7"/>
         <v>WENO</v>
       </c>
-      <c r="Q10" s="41">
-        <f t="shared" si="6"/>
+      <c r="S10" s="25">
+        <f t="shared" si="8"/>
         <v>537.72</v>
       </c>
-      <c r="R10" s="42">
-        <f t="shared" si="7"/>
+      <c r="T10" s="26">
+        <f t="shared" si="9"/>
         <v>415.36000000000007</v>
       </c>
-      <c r="U10" s="23">
+      <c r="W10" s="10">
         <v>2</v>
       </c>
-      <c r="V10" s="24">
+      <c r="X10" s="11">
         <v>6.5590000000000002</v>
       </c>
-      <c r="W10" s="23">
+      <c r="Y10" s="10">
         <v>2.2999999999999998</v>
       </c>
-      <c r="X10" s="24">
+      <c r="Z10" s="11">
         <v>6.5389999999999997</v>
       </c>
-      <c r="Y10" s="23"/>
-      <c r="Z10" s="24"/>
-      <c r="AA10" s="23"/>
-      <c r="AB10" s="24"/>
-      <c r="AC10" s="23"/>
-      <c r="AD10" s="24"/>
+      <c r="AA10" s="10"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="10"/>
+      <c r="AD10" s="11"/>
+      <c r="AE10" s="10"/>
+      <c r="AF10" s="11"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="45">
+      <c r="D11" s="29">
         <f>D2</f>
         <v>410.4</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="52">
         <v>15</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H11" s="25">
-        <f t="shared" si="8"/>
+      <c r="H11" s="53">
+        <f t="shared" si="10"/>
         <v>369.36</v>
       </c>
-      <c r="I11" s="32">
+      <c r="I11" s="18">
         <f t="shared" si="2"/>
         <v>61.86</v>
       </c>
-      <c r="J11" s="33">
+      <c r="J11" s="14">
         <f t="shared" si="3"/>
         <v>53.12</v>
       </c>
-      <c r="K11" s="61">
-        <v>0.2</v>
-      </c>
-      <c r="L11" s="62">
-        <v>0.2</v>
-      </c>
-      <c r="M11" s="32">
+      <c r="K11" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="L11" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="M11" s="13">
         <f t="shared" si="0"/>
         <v>866.04</v>
       </c>
-      <c r="N11" s="33">
+      <c r="N11" s="18">
         <f t="shared" si="4"/>
         <v>743.68000000000006</v>
       </c>
-      <c r="O11" s="24" t="str">
+      <c r="O11" s="38">
         <f t="shared" si="5"/>
+        <v>0.42649300263267287</v>
+      </c>
+      <c r="P11" s="40">
+        <f t="shared" si="6"/>
+        <v>0.49666523235800342</v>
+      </c>
+      <c r="Q11" s="11" t="str">
+        <f t="shared" si="7"/>
         <v>WENO</v>
       </c>
-      <c r="Q11" s="41">
-        <f t="shared" si="6"/>
+      <c r="S11" s="25">
+        <f t="shared" si="8"/>
         <v>496.67999999999995</v>
       </c>
-      <c r="R11" s="42">
-        <f t="shared" si="7"/>
+      <c r="T11" s="26">
+        <f t="shared" si="9"/>
         <v>374.32000000000005</v>
       </c>
-      <c r="U11" s="23"/>
-      <c r="V11" s="24">
+      <c r="W11" s="10"/>
+      <c r="X11" s="11">
         <v>6.359</v>
       </c>
-      <c r="W11" s="23">
+      <c r="Y11" s="10">
         <v>4.7300000000000004</v>
       </c>
-      <c r="X11" s="24">
+      <c r="Z11" s="11">
         <v>5.4</v>
       </c>
-      <c r="Y11" s="23"/>
-      <c r="Z11" s="24"/>
-      <c r="AA11" s="23"/>
-      <c r="AB11" s="24"/>
-      <c r="AC11" s="23"/>
-      <c r="AD11" s="24"/>
+      <c r="AA11" s="10"/>
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="10"/>
+      <c r="AD11" s="11"/>
+      <c r="AE11" s="10"/>
+      <c r="AF11" s="11"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
-      <c r="B12" s="50"/>
+      <c r="B12" s="34"/>
       <c r="C12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="6">
         <v>-55.494999999999997</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="52">
         <v>14</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H12" s="25">
-        <f t="shared" si="8"/>
+      <c r="H12" s="53">
+        <f t="shared" si="10"/>
         <v>410.40000000000003</v>
       </c>
-      <c r="I12" s="32">
+      <c r="I12" s="18">
         <f t="shared" si="2"/>
         <v>61.86</v>
       </c>
-      <c r="J12" s="33">
+      <c r="J12" s="14">
         <f t="shared" si="3"/>
         <v>53.12</v>
       </c>
-      <c r="K12" s="61">
-        <v>0.2</v>
-      </c>
-      <c r="L12" s="62">
-        <v>0.2</v>
-      </c>
-      <c r="M12" s="32">
+      <c r="K12" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="L12" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="M12" s="13">
         <f t="shared" si="0"/>
         <v>866.04</v>
       </c>
-      <c r="N12" s="33">
+      <c r="N12" s="18">
         <f t="shared" si="4"/>
         <v>743.68000000000006</v>
       </c>
-      <c r="O12" s="24" t="str">
+      <c r="O12" s="38">
         <f t="shared" si="5"/>
+        <v>0.47388111403630323</v>
+      </c>
+      <c r="P12" s="40">
+        <f t="shared" si="6"/>
+        <v>0.55185025817555933</v>
+      </c>
+      <c r="Q12" s="11" t="str">
+        <f t="shared" si="7"/>
         <v>WENO</v>
       </c>
-      <c r="Q12" s="41">
-        <f t="shared" si="6"/>
+      <c r="S12" s="25">
+        <f t="shared" si="8"/>
         <v>455.63999999999993</v>
       </c>
-      <c r="R12" s="42">
-        <f t="shared" si="7"/>
+      <c r="T12" s="26">
+        <f t="shared" si="9"/>
         <v>333.28000000000003</v>
       </c>
-      <c r="U12" s="23">
+      <c r="W12" s="10">
         <v>4.05</v>
       </c>
-      <c r="V12" s="24">
+      <c r="X12" s="11">
         <v>5.4</v>
       </c>
-      <c r="W12" s="23">
+      <c r="Y12" s="10">
         <v>2</v>
       </c>
-      <c r="X12" s="24">
+      <c r="Z12" s="11">
         <v>6.5590000000000002</v>
       </c>
-      <c r="Y12" s="23"/>
-      <c r="Z12" s="24"/>
-      <c r="AA12" s="23"/>
-      <c r="AB12" s="24"/>
-      <c r="AC12" s="23"/>
-      <c r="AD12" s="24"/>
+      <c r="AA12" s="10"/>
+      <c r="AB12" s="11"/>
+      <c r="AC12" s="10"/>
+      <c r="AD12" s="11"/>
+      <c r="AE12" s="10"/>
+      <c r="AF12" s="11"/>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
-      <c r="B13" s="50"/>
+      <c r="B13" s="34"/>
       <c r="C13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="6">
         <v>-28.218</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="52">
         <v>13</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H13" s="25">
-        <f t="shared" si="8"/>
+      <c r="H13" s="53">
+        <f t="shared" si="10"/>
         <v>451.44000000000005</v>
       </c>
-      <c r="I13" s="32">
+      <c r="I13" s="18">
         <f t="shared" si="2"/>
         <v>61.86</v>
       </c>
-      <c r="J13" s="33">
+      <c r="J13" s="14">
         <f t="shared" si="3"/>
         <v>53.12</v>
       </c>
-      <c r="K13" s="61">
-        <v>0.2</v>
-      </c>
-      <c r="L13" s="62">
-        <v>0.2</v>
-      </c>
-      <c r="M13" s="32">
+      <c r="K13" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="L13" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="M13" s="13">
         <f t="shared" si="0"/>
         <v>866.04</v>
       </c>
-      <c r="N13" s="33">
+      <c r="N13" s="18">
         <f t="shared" si="4"/>
         <v>743.68000000000006</v>
       </c>
-      <c r="O13" s="24" t="str">
+      <c r="O13" s="38">
         <f t="shared" si="5"/>
+        <v>0.52126922543993359</v>
+      </c>
+      <c r="P13" s="40">
+        <f t="shared" si="6"/>
+        <v>0.60703528399311535</v>
+      </c>
+      <c r="Q13" s="11" t="str">
+        <f t="shared" si="7"/>
         <v>WENO</v>
       </c>
-      <c r="Q13" s="41">
-        <f t="shared" si="6"/>
+      <c r="S13" s="25">
+        <f t="shared" si="8"/>
         <v>414.59999999999991</v>
       </c>
-      <c r="R13" s="42">
-        <f t="shared" si="7"/>
+      <c r="T13" s="26">
+        <f t="shared" si="9"/>
         <v>292.24</v>
       </c>
-      <c r="U13" s="23">
+      <c r="W13" s="10">
         <v>4.7300000000000004</v>
       </c>
-      <c r="V13" s="24">
+      <c r="X13" s="11">
         <v>6.5430000000000001</v>
       </c>
-      <c r="W13" s="23">
+      <c r="Y13" s="10">
         <v>4.5999999999999996</v>
       </c>
-      <c r="X13" s="24">
+      <c r="Z13" s="11">
         <v>6.359</v>
       </c>
-      <c r="Y13" s="23"/>
-      <c r="Z13" s="24"/>
-      <c r="AA13" s="23"/>
-      <c r="AB13" s="24"/>
-      <c r="AC13" s="23"/>
-      <c r="AD13" s="24"/>
+      <c r="AA13" s="10"/>
+      <c r="AB13" s="11"/>
+      <c r="AC13" s="10"/>
+      <c r="AD13" s="11"/>
+      <c r="AE13" s="10"/>
+      <c r="AF13" s="11"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
-      <c r="B14" s="50"/>
+      <c r="B14" s="34"/>
       <c r="C14" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="8">
-        <v>280.947</v>
-      </c>
-      <c r="F14" s="10">
+      <c r="D14" s="6">
+        <f>280.947/2</f>
+        <v>140.4735</v>
+      </c>
+      <c r="F14" s="52">
         <v>12</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H14" s="25">
-        <f t="shared" si="8"/>
+      <c r="H14" s="53">
+        <f t="shared" si="10"/>
         <v>492.48000000000008</v>
       </c>
-      <c r="I14" s="32">
+      <c r="I14" s="18">
         <f t="shared" si="2"/>
         <v>61.86</v>
       </c>
-      <c r="J14" s="33">
+      <c r="J14" s="14">
         <f t="shared" si="3"/>
         <v>53.12</v>
       </c>
-      <c r="K14" s="61">
-        <v>0.2</v>
-      </c>
-      <c r="L14" s="62">
-        <v>0.2</v>
-      </c>
-      <c r="M14" s="32">
+      <c r="K14" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="L14" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="M14" s="13">
         <f t="shared" si="0"/>
         <v>866.04</v>
       </c>
-      <c r="N14" s="33">
+      <c r="N14" s="18">
         <f t="shared" si="4"/>
         <v>743.68000000000006</v>
       </c>
-      <c r="O14" s="24" t="str">
+      <c r="O14" s="38">
         <f t="shared" si="5"/>
+        <v>0.5686573368435639</v>
+      </c>
+      <c r="P14" s="40">
+        <f t="shared" si="6"/>
+        <v>0.66222030981067126</v>
+      </c>
+      <c r="Q14" s="11" t="str">
+        <f t="shared" si="7"/>
         <v>WENO</v>
       </c>
-      <c r="Q14" s="41">
-        <f t="shared" si="6"/>
+      <c r="S14" s="25">
+        <f t="shared" si="8"/>
         <v>373.55999999999989</v>
       </c>
-      <c r="R14" s="42">
-        <f t="shared" si="7"/>
+      <c r="T14" s="26">
+        <f t="shared" si="9"/>
         <v>251.2</v>
       </c>
-      <c r="U14" s="23"/>
-      <c r="V14" s="24">
+      <c r="W14" s="10"/>
+      <c r="X14" s="11">
         <v>1.92</v>
       </c>
-      <c r="W14" s="23">
+      <c r="Y14" s="10">
         <v>5.5</v>
       </c>
-      <c r="X14" s="24">
+      <c r="Z14" s="11">
         <v>1.92</v>
       </c>
-      <c r="Y14" s="23"/>
-      <c r="Z14" s="24"/>
-      <c r="AA14" s="23"/>
-      <c r="AB14" s="24"/>
-      <c r="AC14" s="23"/>
-      <c r="AD14" s="24"/>
+      <c r="AA14" s="10"/>
+      <c r="AB14" s="11"/>
+      <c r="AC14" s="10"/>
+      <c r="AD14" s="11"/>
+      <c r="AE14" s="10"/>
+      <c r="AF14" s="11"/>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
-      <c r="B15" s="50"/>
+      <c r="B15" s="34"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="8"/>
-      <c r="F15" s="10">
+      <c r="D15" s="6"/>
+      <c r="F15" s="52">
         <v>11</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H15" s="25">
-        <f t="shared" si="8"/>
+      <c r="H15" s="53">
+        <f t="shared" si="10"/>
         <v>533.5200000000001</v>
       </c>
-      <c r="I15" s="32">
+      <c r="I15" s="18">
         <f t="shared" si="2"/>
         <v>61.86</v>
       </c>
-      <c r="J15" s="33">
+      <c r="J15" s="14">
         <f t="shared" si="3"/>
         <v>53.12</v>
       </c>
-      <c r="K15" s="61">
-        <v>0.2</v>
-      </c>
-      <c r="L15" s="62">
-        <v>0.2</v>
-      </c>
-      <c r="M15" s="32">
+      <c r="K15" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="L15" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="M15" s="13">
         <f t="shared" si="0"/>
         <v>866.04</v>
       </c>
-      <c r="N15" s="33">
+      <c r="N15" s="18">
         <f t="shared" si="4"/>
         <v>743.68000000000006</v>
       </c>
-      <c r="O15" s="24" t="str">
+      <c r="O15" s="38">
         <f t="shared" si="5"/>
+        <v>0.61604544824719432</v>
+      </c>
+      <c r="P15" s="40">
+        <f t="shared" si="6"/>
+        <v>0.71740533562822728</v>
+      </c>
+      <c r="Q15" s="11" t="str">
+        <f t="shared" si="7"/>
         <v>WENO</v>
       </c>
-      <c r="Q15" s="41">
-        <f t="shared" si="6"/>
+      <c r="S15" s="25">
+        <f t="shared" si="8"/>
         <v>332.51999999999987</v>
       </c>
-      <c r="R15" s="42">
-        <f t="shared" si="7"/>
+      <c r="T15" s="26">
+        <f t="shared" si="9"/>
         <v>210.15999999999997</v>
       </c>
-      <c r="U15" s="23">
+      <c r="W15" s="10">
         <v>5.46</v>
       </c>
-      <c r="V15" s="24">
+      <c r="X15" s="11">
         <v>3.39</v>
       </c>
-      <c r="W15" s="23">
+      <c r="Y15" s="10">
         <v>3.08</v>
       </c>
-      <c r="X15" s="24">
+      <c r="Z15" s="11">
         <v>3.39</v>
       </c>
-      <c r="Y15" s="23"/>
-      <c r="Z15" s="24"/>
-      <c r="AA15" s="23"/>
-      <c r="AB15" s="24"/>
-      <c r="AC15" s="23"/>
-      <c r="AD15" s="24"/>
+      <c r="AA15" s="10"/>
+      <c r="AB15" s="11"/>
+      <c r="AC15" s="10"/>
+      <c r="AD15" s="11"/>
+      <c r="AE15" s="10"/>
+      <c r="AF15" s="11"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
-      <c r="B16" s="50"/>
+      <c r="B16" s="34"/>
       <c r="C16" s="4"/>
-      <c r="D16" s="8"/>
-      <c r="F16" s="10">
+      <c r="D16" s="6"/>
+      <c r="F16" s="52">
         <v>10</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H16" s="25">
-        <f t="shared" si="8"/>
+      <c r="H16" s="53">
+        <f t="shared" si="10"/>
         <v>574.56000000000006</v>
       </c>
-      <c r="I16" s="32">
+      <c r="I16" s="18">
         <f t="shared" si="2"/>
         <v>61.86</v>
       </c>
-      <c r="J16" s="33">
+      <c r="J16" s="14">
         <f t="shared" si="3"/>
         <v>53.12</v>
       </c>
-      <c r="K16" s="61">
-        <v>0.2</v>
-      </c>
-      <c r="L16" s="62">
-        <v>0.2</v>
-      </c>
-      <c r="M16" s="32">
+      <c r="K16" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="L16" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="M16" s="13">
         <f t="shared" si="0"/>
         <v>866.04</v>
       </c>
-      <c r="N16" s="33">
+      <c r="N16" s="18">
         <f t="shared" si="4"/>
         <v>743.68000000000006</v>
       </c>
-      <c r="O16" s="24" t="str">
+      <c r="O16" s="38">
         <f t="shared" si="5"/>
+        <v>0.66343355965082451</v>
+      </c>
+      <c r="P16" s="40">
+        <f t="shared" si="6"/>
+        <v>0.77259036144578319</v>
+      </c>
+      <c r="Q16" s="11" t="str">
+        <f t="shared" si="7"/>
         <v>WENO</v>
       </c>
-      <c r="Q16" s="41">
-        <f t="shared" si="6"/>
+      <c r="S16" s="25">
+        <f t="shared" si="8"/>
         <v>291.4799999999999</v>
       </c>
-      <c r="R16" s="42">
-        <f t="shared" si="7"/>
+      <c r="T16" s="26">
+        <f t="shared" si="9"/>
         <v>169.12</v>
       </c>
-      <c r="U16" s="23">
+      <c r="W16" s="10">
         <v>2.2999999999999998</v>
       </c>
-      <c r="V16" s="24">
+      <c r="X16" s="11">
         <v>1.6</v>
       </c>
-      <c r="W16" s="23"/>
-      <c r="X16" s="24">
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="11">
         <v>3.39</v>
       </c>
-      <c r="Y16" s="23"/>
-      <c r="Z16" s="24"/>
-      <c r="AA16" s="23"/>
-      <c r="AB16" s="24"/>
-      <c r="AC16" s="23"/>
-      <c r="AD16" s="24"/>
+      <c r="AA16" s="10"/>
+      <c r="AB16" s="11"/>
+      <c r="AC16" s="10"/>
+      <c r="AD16" s="11"/>
+      <c r="AE16" s="10"/>
+      <c r="AF16" s="11"/>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
-      <c r="B17" s="50"/>
+      <c r="B17" s="34"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="8"/>
-      <c r="F17" s="10">
+      <c r="D17" s="6"/>
+      <c r="F17" s="52">
         <v>9</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H17" s="25">
-        <f t="shared" si="8"/>
+      <c r="H17" s="53">
+        <f t="shared" si="10"/>
         <v>615.6</v>
       </c>
-      <c r="I17" s="32">
+      <c r="I17" s="18">
         <f t="shared" si="2"/>
         <v>61.86</v>
       </c>
-      <c r="J17" s="33">
+      <c r="J17" s="14">
         <f t="shared" si="3"/>
         <v>53.12</v>
       </c>
-      <c r="K17" s="61">
-        <v>0.2</v>
-      </c>
-      <c r="L17" s="62">
-        <v>0.2</v>
-      </c>
-      <c r="M17" s="32">
+      <c r="K17" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="L17" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="M17" s="13">
         <f t="shared" si="0"/>
         <v>866.04</v>
       </c>
-      <c r="N17" s="33">
+      <c r="N17" s="18">
         <f t="shared" si="4"/>
         <v>743.68000000000006</v>
       </c>
-      <c r="O17" s="24" t="str">
+      <c r="O17" s="38">
         <f t="shared" si="5"/>
+        <v>0.71082167105445482</v>
+      </c>
+      <c r="P17" s="40">
+        <f t="shared" si="6"/>
+        <v>0.82777538726333899</v>
+      </c>
+      <c r="Q17" s="11" t="str">
+        <f t="shared" si="7"/>
         <v>WENO</v>
       </c>
-      <c r="Q17" s="41">
-        <f t="shared" si="6"/>
+      <c r="S17" s="25">
+        <f t="shared" si="8"/>
         <v>250.43999999999994</v>
       </c>
-      <c r="R17" s="42">
-        <f t="shared" si="7"/>
+      <c r="T17" s="26">
+        <f t="shared" si="9"/>
         <v>128.08000000000004</v>
       </c>
-      <c r="U17" s="23">
+      <c r="W17" s="10">
         <v>2</v>
       </c>
-      <c r="V17" s="24">
+      <c r="X17" s="11">
         <v>3.35</v>
       </c>
-      <c r="W17" s="23"/>
-      <c r="X17" s="24">
+      <c r="Y17" s="10"/>
+      <c r="Z17" s="11">
         <v>1.6</v>
       </c>
-      <c r="Y17" s="23"/>
-      <c r="Z17" s="24"/>
-      <c r="AA17" s="23"/>
-      <c r="AB17" s="24"/>
-      <c r="AC17" s="23"/>
-      <c r="AD17" s="24"/>
+      <c r="AA17" s="10"/>
+      <c r="AB17" s="11"/>
+      <c r="AC17" s="10"/>
+      <c r="AD17" s="11"/>
+      <c r="AE17" s="10"/>
+      <c r="AF17" s="11"/>
     </row>
-    <row r="18" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="52" t="s">
+      <c r="B18" s="35"/>
+      <c r="C18" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="7">
         <f>SUM(D11:D14)</f>
-        <v>607.63400000000001</v>
-      </c>
-      <c r="F18" s="10">
+        <v>467.16049999999996</v>
+      </c>
+      <c r="F18" s="52">
         <v>8</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H18" s="25">
-        <f t="shared" si="8"/>
+      <c r="H18" s="53">
+        <f t="shared" si="10"/>
         <v>656.64</v>
       </c>
-      <c r="I18" s="32">
+      <c r="I18" s="18">
         <f t="shared" si="2"/>
         <v>61.86</v>
       </c>
-      <c r="J18" s="33">
+      <c r="J18" s="14">
         <f t="shared" si="3"/>
         <v>53.12</v>
       </c>
-      <c r="K18" s="61">
-        <v>0.2</v>
-      </c>
-      <c r="L18" s="62">
-        <v>0.2</v>
-      </c>
-      <c r="M18" s="32">
+      <c r="K18" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="L18" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="M18" s="13">
         <f t="shared" si="0"/>
         <v>866.04</v>
       </c>
-      <c r="N18" s="33">
+      <c r="N18" s="18">
         <f t="shared" si="4"/>
         <v>743.68000000000006</v>
       </c>
-      <c r="O18" s="24" t="str">
+      <c r="O18" s="38">
         <f t="shared" si="5"/>
+        <v>0.75820978245808512</v>
+      </c>
+      <c r="P18" s="40">
+        <f t="shared" si="6"/>
+        <v>0.8829604130808949</v>
+      </c>
+      <c r="Q18" s="11" t="str">
+        <f t="shared" si="7"/>
         <v>WENO</v>
       </c>
-      <c r="Q18" s="41">
-        <f t="shared" si="6"/>
+      <c r="S18" s="25">
+        <f t="shared" si="8"/>
         <v>209.39999999999998</v>
       </c>
-      <c r="R18" s="42">
-        <f t="shared" si="7"/>
+      <c r="T18" s="26">
+        <f t="shared" si="9"/>
         <v>87.040000000000077</v>
       </c>
-      <c r="U18" s="23"/>
-      <c r="V18" s="24">
+      <c r="W18" s="10"/>
+      <c r="X18" s="11">
         <v>1.92</v>
       </c>
-      <c r="W18" s="23"/>
-      <c r="X18" s="24"/>
-      <c r="Y18" s="23"/>
-      <c r="Z18" s="24"/>
-      <c r="AA18" s="23"/>
-      <c r="AB18" s="24"/>
-      <c r="AC18" s="23"/>
-      <c r="AD18" s="24"/>
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="10"/>
+      <c r="AB18" s="11"/>
+      <c r="AC18" s="10"/>
+      <c r="AD18" s="11"/>
+      <c r="AE18" s="10"/>
+      <c r="AF18" s="11"/>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
-      <c r="B19" s="53"/>
+      <c r="B19" s="37"/>
       <c r="C19" s="4"/>
       <c r="D19" s="5"/>
-      <c r="F19" s="10">
+      <c r="F19" s="52">
         <v>7</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H19" s="25">
-        <f t="shared" si="8"/>
+      <c r="H19" s="53">
+        <f t="shared" si="10"/>
         <v>697.68</v>
       </c>
-      <c r="I19" s="32">
+      <c r="I19" s="18">
         <f t="shared" si="2"/>
         <v>61.86</v>
       </c>
-      <c r="J19" s="33">
+      <c r="J19" s="14">
         <f t="shared" si="3"/>
         <v>53.12</v>
       </c>
-      <c r="K19" s="61">
-        <v>0.2</v>
-      </c>
-      <c r="L19" s="62">
-        <v>0.2</v>
-      </c>
-      <c r="M19" s="32">
+      <c r="K19" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="L19" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="M19" s="13">
         <f t="shared" si="0"/>
         <v>866.04</v>
       </c>
-      <c r="N19" s="33">
+      <c r="N19" s="18">
         <f t="shared" si="4"/>
         <v>743.68000000000006</v>
       </c>
-      <c r="O19" s="24" t="str">
+      <c r="O19" s="38">
         <f t="shared" si="5"/>
+        <v>0.80559789386171532</v>
+      </c>
+      <c r="P19" s="40">
+        <f t="shared" si="6"/>
+        <v>0.93814543889845081</v>
+      </c>
+      <c r="Q19" s="11" t="str">
+        <f t="shared" si="7"/>
         <v>WENO</v>
       </c>
-      <c r="Q19" s="41">
-        <f t="shared" si="6"/>
+      <c r="S19" s="25">
+        <f t="shared" si="8"/>
         <v>168.36</v>
       </c>
-      <c r="R19" s="42">
-        <f t="shared" si="7"/>
+      <c r="T19" s="26">
+        <f t="shared" si="9"/>
         <v>46.000000000000114</v>
       </c>
-      <c r="U19" s="23">
+      <c r="W19" s="10">
         <v>4.5999999999999996</v>
       </c>
-      <c r="V19" s="24">
+      <c r="X19" s="11">
         <v>1.6</v>
       </c>
-      <c r="W19" s="23"/>
-      <c r="X19" s="24"/>
-      <c r="Y19" s="23"/>
-      <c r="Z19" s="24"/>
-      <c r="AA19" s="23"/>
-      <c r="AB19" s="24"/>
-      <c r="AC19" s="23"/>
-      <c r="AD19" s="24"/>
+      <c r="Y19" s="10"/>
+      <c r="Z19" s="11"/>
+      <c r="AA19" s="10"/>
+      <c r="AB19" s="11"/>
+      <c r="AC19" s="10"/>
+      <c r="AD19" s="11"/>
+      <c r="AE19" s="10"/>
+      <c r="AF19" s="11"/>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
-      <c r="B20" s="53" t="s">
+      <c r="B20" s="37" t="s">
         <v>40</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -2366,67 +2421,75 @@
       <c r="D20" s="4">
         <v>1066.5999999999999</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="52">
         <v>6</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H20" s="25">
-        <f t="shared" si="8"/>
+      <c r="H20" s="53">
+        <f t="shared" si="10"/>
         <v>738.71999999999991</v>
       </c>
-      <c r="I20" s="32">
+      <c r="I20" s="18">
         <f t="shared" si="2"/>
         <v>61.86</v>
       </c>
-      <c r="J20" s="33">
+      <c r="J20" s="14">
         <f t="shared" si="3"/>
         <v>53.12</v>
       </c>
-      <c r="K20" s="61">
-        <v>0.2</v>
-      </c>
-      <c r="L20" s="62">
-        <v>0.2</v>
-      </c>
-      <c r="M20" s="32">
+      <c r="K20" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="L20" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="M20" s="13">
         <f t="shared" si="0"/>
         <v>866.04</v>
       </c>
-      <c r="N20" s="33">
+      <c r="N20" s="18">
         <f t="shared" si="4"/>
         <v>743.68000000000006</v>
       </c>
-      <c r="O20" s="24" t="str">
+      <c r="O20" s="38">
         <f t="shared" si="5"/>
+        <v>0.85298600526534563</v>
+      </c>
+      <c r="P20" s="40">
+        <f t="shared" si="6"/>
+        <v>0.99333046471600672</v>
+      </c>
+      <c r="Q20" s="11" t="str">
+        <f t="shared" si="7"/>
         <v>WENO</v>
       </c>
-      <c r="Q20" s="41">
-        <f t="shared" si="6"/>
+      <c r="S20" s="25">
+        <f t="shared" si="8"/>
         <v>127.32000000000005</v>
       </c>
-      <c r="R20" s="42">
-        <f t="shared" si="7"/>
+      <c r="T20" s="26">
+        <f t="shared" si="9"/>
         <v>4.9600000000001501</v>
       </c>
-      <c r="U20" s="23">
+      <c r="W20" s="10">
         <v>5.5</v>
       </c>
-      <c r="V20" s="24"/>
-      <c r="W20" s="23"/>
-      <c r="X20" s="24"/>
-      <c r="Y20" s="23"/>
-      <c r="Z20" s="24"/>
-      <c r="AA20" s="23"/>
-      <c r="AB20" s="24"/>
-      <c r="AC20" s="23"/>
-      <c r="AD20" s="24"/>
+      <c r="X20" s="11"/>
+      <c r="Y20" s="10"/>
+      <c r="Z20" s="11"/>
+      <c r="AA20" s="10"/>
+      <c r="AB20" s="11"/>
+      <c r="AC20" s="10"/>
+      <c r="AD20" s="11"/>
+      <c r="AE20" s="10"/>
+      <c r="AF20" s="11"/>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
-      <c r="B21" s="53"/>
+      <c r="B21" s="37"/>
       <c r="C21" s="4" t="s">
         <v>44</v>
       </c>
@@ -2434,65 +2497,73 @@
         <f>-7.68</f>
         <v>-7.68</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="52">
         <v>5</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H21" s="25">
-        <f t="shared" si="8"/>
+      <c r="H21" s="53">
+        <f t="shared" si="10"/>
         <v>779.75999999999988</v>
       </c>
-      <c r="I21" s="32">
+      <c r="I21" s="18">
         <f t="shared" si="2"/>
         <v>61.86</v>
       </c>
-      <c r="J21" s="33">
+      <c r="J21" s="14">
         <f t="shared" si="3"/>
         <v>53.12</v>
       </c>
-      <c r="K21" s="61">
-        <v>0.2</v>
-      </c>
-      <c r="L21" s="58">
+      <c r="K21" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="L21" s="43">
         <v>0.25</v>
       </c>
-      <c r="M21" s="32">
+      <c r="M21" s="13">
         <f t="shared" si="0"/>
         <v>866.04</v>
       </c>
-      <c r="N21" s="33">
+      <c r="N21" s="18">
         <f t="shared" si="4"/>
         <v>929.59999999999991</v>
       </c>
-      <c r="O21" s="24" t="str">
+      <c r="O21" s="38">
         <f t="shared" si="5"/>
+        <v>0.90037411666897593</v>
+      </c>
+      <c r="P21" s="40">
+        <f t="shared" si="6"/>
+        <v>0.83881239242685024</v>
+      </c>
+      <c r="Q21" s="11" t="str">
+        <f t="shared" si="7"/>
         <v>WENO</v>
       </c>
-      <c r="Q21" s="41">
-        <f t="shared" si="6"/>
+      <c r="S21" s="25">
+        <f t="shared" si="8"/>
         <v>86.280000000000086</v>
       </c>
-      <c r="R21" s="42">
-        <f t="shared" si="7"/>
+      <c r="T21" s="26">
+        <f t="shared" si="9"/>
         <v>149.84000000000003</v>
       </c>
-      <c r="U21" s="23">
+      <c r="W21" s="10">
         <v>3.08</v>
       </c>
-      <c r="V21" s="24"/>
-      <c r="W21" s="23"/>
-      <c r="X21" s="24"/>
-      <c r="Y21" s="23"/>
-      <c r="Z21" s="24"/>
-      <c r="AA21" s="23"/>
-      <c r="AB21" s="24"/>
-      <c r="AC21" s="23"/>
-      <c r="AD21" s="24"/>
+      <c r="X21" s="11"/>
+      <c r="Y21" s="10"/>
+      <c r="Z21" s="11"/>
+      <c r="AA21" s="10"/>
+      <c r="AB21" s="11"/>
+      <c r="AC21" s="10"/>
+      <c r="AD21" s="11"/>
+      <c r="AE21" s="10"/>
+      <c r="AF21" s="11"/>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
       <c r="C22" s="1" t="s">
         <v>45</v>
       </c>
@@ -2500,122 +2571,138 @@
         <f>D20+D21</f>
         <v>1058.9199999999998</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="52">
         <v>4</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H22" s="25">
-        <f t="shared" si="8"/>
+      <c r="H22" s="53">
+        <f t="shared" si="10"/>
         <v>820.79999999999984</v>
       </c>
-      <c r="I22" s="32">
+      <c r="I22" s="18">
         <f t="shared" si="2"/>
         <v>61.86</v>
       </c>
-      <c r="J22" s="33">
+      <c r="J22" s="14">
         <f t="shared" si="3"/>
         <v>53.12</v>
       </c>
-      <c r="K22" s="61">
-        <v>0.2</v>
-      </c>
-      <c r="L22" s="58">
+      <c r="K22" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="L22" s="43">
         <v>0.25</v>
       </c>
-      <c r="M22" s="32">
+      <c r="M22" s="13">
         <f t="shared" si="0"/>
         <v>866.04</v>
       </c>
-      <c r="N22" s="33">
+      <c r="N22" s="18">
         <f t="shared" si="4"/>
         <v>929.59999999999991</v>
       </c>
-      <c r="O22" s="24" t="str">
+      <c r="O22" s="38">
         <f t="shared" si="5"/>
+        <v>0.94776222807260624</v>
+      </c>
+      <c r="P22" s="40">
+        <f t="shared" si="6"/>
+        <v>0.8829604130808949</v>
+      </c>
+      <c r="Q22" s="11" t="str">
+        <f t="shared" si="7"/>
         <v>WENO</v>
       </c>
-      <c r="Q22" s="41">
-        <f t="shared" si="6"/>
+      <c r="S22" s="25">
+        <f t="shared" si="8"/>
         <v>45.240000000000123</v>
       </c>
-      <c r="R22" s="42">
-        <f t="shared" si="7"/>
+      <c r="T22" s="26">
+        <f t="shared" si="9"/>
         <v>108.80000000000007</v>
       </c>
-      <c r="U22" s="23">
+      <c r="W22" s="10">
         <v>3.08</v>
       </c>
-      <c r="V22" s="24"/>
-      <c r="W22" s="23"/>
-      <c r="X22" s="24"/>
-      <c r="Y22" s="23"/>
-      <c r="Z22" s="24"/>
-      <c r="AA22" s="23"/>
-      <c r="AB22" s="24"/>
-      <c r="AC22" s="23"/>
-      <c r="AD22" s="24"/>
+      <c r="X22" s="11"/>
+      <c r="Y22" s="10"/>
+      <c r="Z22" s="11"/>
+      <c r="AA22" s="10"/>
+      <c r="AB22" s="11"/>
+      <c r="AC22" s="10"/>
+      <c r="AD22" s="11"/>
+      <c r="AE22" s="10"/>
+      <c r="AF22" s="11"/>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="F23" s="11">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="F23" s="52">
         <v>3</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H23" s="26">
+      <c r="H23" s="53">
+        <f t="shared" si="10"/>
+        <v>861.8399999999998</v>
+      </c>
+      <c r="I23" s="18">
+        <f>Z25</f>
+        <v>61.86</v>
+      </c>
+      <c r="J23" s="14">
+        <f>Y25</f>
+        <v>50.03</v>
+      </c>
+      <c r="K23" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="L23" s="43">
+        <v>0.25</v>
+      </c>
+      <c r="M23" s="13">
+        <f t="shared" ref="M23:M24" si="11">I23*K23*$D$8*100*100</f>
+        <v>866.04</v>
+      </c>
+      <c r="N23" s="18">
+        <f t="shared" ref="N23:N24" si="12">J23*L23*$D$8*100*100</f>
+        <v>875.52499999999998</v>
+      </c>
+      <c r="O23" s="38">
+        <f t="shared" si="5"/>
+        <v>0.99515033947623643</v>
+      </c>
+      <c r="P23" s="40">
+        <f t="shared" si="6"/>
+        <v>0.984369378372976</v>
+      </c>
+      <c r="Q23" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>WENO</v>
+      </c>
+      <c r="S23" s="25">
         <f t="shared" si="8"/>
-        <v>861.8399999999998</v>
-      </c>
-      <c r="I23" s="32">
-        <f>X25</f>
-        <v>61.86</v>
-      </c>
-      <c r="J23" s="33">
-        <f>W25</f>
-        <v>50.03</v>
-      </c>
-      <c r="K23" s="61">
-        <v>0.2</v>
-      </c>
-      <c r="L23" s="58">
-        <v>0.25</v>
-      </c>
-      <c r="M23" s="32">
-        <f t="shared" ref="M23:M24" si="9">I23*K23*$D$8*100*100</f>
-        <v>866.04</v>
-      </c>
-      <c r="N23" s="33">
-        <f t="shared" ref="N23:N24" si="10">J23*L23*$D$8*100*100</f>
-        <v>875.52499999999998</v>
-      </c>
-      <c r="O23" s="24" t="str">
-        <f t="shared" si="5"/>
-        <v>WENO</v>
-      </c>
-      <c r="Q23" s="41">
-        <f t="shared" si="6"/>
         <v>4.2000000000001592</v>
       </c>
-      <c r="R23" s="42">
-        <f t="shared" si="7"/>
+      <c r="T23" s="26">
+        <f t="shared" si="9"/>
         <v>13.685000000000173</v>
       </c>
-      <c r="U23" s="23"/>
-      <c r="V23" s="24"/>
-      <c r="W23" s="23"/>
-      <c r="X23" s="24"/>
-      <c r="Y23" s="23"/>
-      <c r="Z23" s="24"/>
-      <c r="AA23" s="23"/>
-      <c r="AB23" s="24"/>
-      <c r="AC23" s="23"/>
-      <c r="AD23" s="24"/>
+      <c r="W23" s="10"/>
+      <c r="X23" s="11"/>
+      <c r="Y23" s="10"/>
+      <c r="Z23" s="11"/>
+      <c r="AA23" s="10"/>
+      <c r="AB23" s="11"/>
+      <c r="AC23" s="10"/>
+      <c r="AD23" s="11"/>
+      <c r="AE23" s="10"/>
+      <c r="AF23" s="11"/>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
       <c r="C24" s="3" t="s">
         <v>46</v>
       </c>
@@ -2626,208 +2713,232 @@
       <c r="E24" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="52">
         <v>2</v>
       </c>
-      <c r="G24" s="54">
+      <c r="G24" s="50">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H24" s="27">
+      <c r="H24" s="53">
+        <f t="shared" si="10"/>
+        <v>902.87999999999977</v>
+      </c>
+      <c r="I24" s="18">
+        <f>AB25</f>
+        <v>60.38</v>
+      </c>
+      <c r="J24" s="14">
+        <f>AA25</f>
+        <v>45</v>
+      </c>
+      <c r="K24" s="42">
+        <v>0.25</v>
+      </c>
+      <c r="L24" s="47">
+        <v>0.3</v>
+      </c>
+      <c r="M24" s="13">
+        <f t="shared" si="11"/>
+        <v>1056.6500000000001</v>
+      </c>
+      <c r="N24" s="18">
+        <f t="shared" si="12"/>
+        <v>944.99999999999989</v>
+      </c>
+      <c r="O24" s="38">
+        <f t="shared" si="5"/>
+        <v>0.85447404533194504</v>
+      </c>
+      <c r="P24" s="40">
+        <f t="shared" si="6"/>
+        <v>0.95542857142857129</v>
+      </c>
+      <c r="Q24" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>WENO</v>
+      </c>
+      <c r="S24" s="25">
         <f t="shared" si="8"/>
-        <v>902.87999999999977</v>
-      </c>
-      <c r="I24" s="32">
-        <f>Z25</f>
-        <v>60.38</v>
-      </c>
-      <c r="J24" s="33">
-        <f>Y25</f>
-        <v>45</v>
-      </c>
-      <c r="K24" s="56">
-        <v>0.25</v>
-      </c>
-      <c r="L24" s="59">
-        <v>0.3</v>
-      </c>
-      <c r="M24" s="32">
+        <v>153.77000000000032</v>
+      </c>
+      <c r="T24" s="26">
         <f t="shared" si="9"/>
-        <v>1056.6500000000001</v>
-      </c>
-      <c r="N24" s="33">
-        <f t="shared" si="10"/>
-        <v>944.99999999999989</v>
-      </c>
-      <c r="O24" s="24" t="str">
-        <f t="shared" si="5"/>
-        <v>WENO</v>
-      </c>
-      <c r="Q24" s="41">
-        <f t="shared" si="6"/>
-        <v>153.77000000000032</v>
-      </c>
-      <c r="R24" s="42">
-        <f t="shared" si="7"/>
         <v>42.120000000000118</v>
       </c>
-      <c r="U24" s="23"/>
-      <c r="V24" s="24"/>
-      <c r="W24" s="23"/>
-      <c r="X24" s="24"/>
-      <c r="Y24" s="23"/>
-      <c r="Z24" s="24"/>
-      <c r="AA24" s="23"/>
-      <c r="AB24" s="24"/>
-      <c r="AC24" s="23"/>
-      <c r="AD24" s="24"/>
+      <c r="W24" s="10"/>
+      <c r="X24" s="11"/>
+      <c r="Y24" s="10"/>
+      <c r="Z24" s="11"/>
+      <c r="AA24" s="10"/>
+      <c r="AB24" s="11"/>
+      <c r="AC24" s="10"/>
+      <c r="AD24" s="11"/>
+      <c r="AE24" s="10"/>
+      <c r="AF24" s="11"/>
     </row>
-    <row r="25" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E25" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="13">
+      <c r="F25" s="52">
         <v>1</v>
       </c>
-      <c r="G25" s="55">
+      <c r="G25" s="51">
         <f>$D$18*$D$4*$D$5</f>
-        <v>60.763400000000004</v>
-      </c>
-      <c r="H25" s="28">
+        <v>46.716049999999996</v>
+      </c>
+      <c r="H25" s="53">
+        <f t="shared" si="10"/>
+        <v>949.59604999999976</v>
+      </c>
+      <c r="I25" s="18">
+        <f>AD25</f>
+        <v>71.489999999999995</v>
+      </c>
+      <c r="J25" s="14">
+        <f>AC25</f>
+        <v>48.88</v>
+      </c>
+      <c r="K25" s="42">
+        <v>0.25</v>
+      </c>
+      <c r="L25" s="47">
+        <v>0.3</v>
+      </c>
+      <c r="M25" s="13">
+        <f t="shared" ref="M25" si="13">I25*K25*$D$8*100*100</f>
+        <v>1251.0749999999998</v>
+      </c>
+      <c r="N25" s="18">
+        <f t="shared" ref="N25" si="14">J25*L25*$D$8*100*100</f>
+        <v>1026.48</v>
+      </c>
+      <c r="O25" s="38">
+        <f t="shared" si="5"/>
+        <v>0.75902407929180893</v>
+      </c>
+      <c r="P25" s="40">
+        <f t="shared" si="6"/>
+        <v>0.92509941742654489</v>
+      </c>
+      <c r="Q25" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>WENO</v>
+      </c>
+      <c r="R25" t="s">
+        <v>13</v>
+      </c>
+      <c r="S25" s="25">
         <f t="shared" si="8"/>
-        <v>963.64339999999982</v>
-      </c>
-      <c r="I25" s="32">
-        <f>AB25</f>
+        <v>301.47895000000005</v>
+      </c>
+      <c r="T25" s="26">
+        <f t="shared" si="9"/>
+        <v>76.883950000000254</v>
+      </c>
+      <c r="V25" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="W25" s="30">
+        <v>53.12</v>
+      </c>
+      <c r="X25" s="31">
+        <v>61.86</v>
+      </c>
+      <c r="Y25" s="30">
+        <v>50.03</v>
+      </c>
+      <c r="Z25" s="31">
+        <v>61.86</v>
+      </c>
+      <c r="AA25" s="30">
+        <v>45</v>
+      </c>
+      <c r="AB25" s="31">
+        <v>60.38</v>
+      </c>
+      <c r="AC25" s="30">
+        <v>48.88</v>
+      </c>
+      <c r="AD25" s="31">
         <v>71.489999999999995</v>
       </c>
-      <c r="J25" s="33">
-        <f>AA25</f>
-        <v>48.88</v>
-      </c>
-      <c r="K25" s="56">
-        <v>0.25</v>
-      </c>
-      <c r="L25" s="59">
-        <v>0.3</v>
-      </c>
-      <c r="M25" s="32">
-        <f t="shared" ref="M25" si="11">I25*K25*$D$8*100*100</f>
-        <v>1251.0749999999998</v>
-      </c>
-      <c r="N25" s="33">
-        <f t="shared" ref="N25" si="12">J25*L25*$D$8*100*100</f>
-        <v>1026.48</v>
-      </c>
-      <c r="O25" s="24" t="str">
-        <f t="shared" si="5"/>
-        <v>WENO</v>
-      </c>
-      <c r="P25" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q25" s="41">
-        <f t="shared" si="6"/>
-        <v>287.4316</v>
-      </c>
-      <c r="R25" s="42">
-        <f t="shared" si="7"/>
-        <v>62.836600000000203</v>
-      </c>
-      <c r="T25" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="U25" s="46">
-        <v>53.12</v>
-      </c>
-      <c r="V25" s="47">
-        <v>61.86</v>
-      </c>
-      <c r="W25" s="46">
-        <v>50.03</v>
-      </c>
-      <c r="X25" s="47">
-        <v>61.86</v>
-      </c>
-      <c r="Y25" s="46">
-        <v>45</v>
-      </c>
-      <c r="Z25" s="47">
-        <v>60.38</v>
-      </c>
-      <c r="AA25" s="46">
-        <v>48.88</v>
-      </c>
-      <c r="AB25" s="47">
-        <v>71.489999999999995</v>
-      </c>
-      <c r="AC25" s="46">
+      <c r="AE25" s="30">
         <v>50.55</v>
       </c>
-      <c r="AD25" s="47">
+      <c r="AF25" s="31">
         <v>94.19</v>
       </c>
     </row>
-    <row r="26" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E26" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="14">
+      <c r="F26" s="54">
         <v>-1</v>
       </c>
-      <c r="G26" s="29">
+      <c r="G26" s="55">
         <f>$D$24*$D$4*$D$5</f>
         <v>73.465999999999994</v>
       </c>
-      <c r="H26" s="30">
+      <c r="H26" s="56">
+        <f t="shared" si="10"/>
+        <v>1023.0620499999998</v>
+      </c>
+      <c r="I26" s="20">
+        <f>AF25</f>
+        <v>94.19</v>
+      </c>
+      <c r="J26" s="16">
+        <f>AE25</f>
+        <v>50.55</v>
+      </c>
+      <c r="K26" s="46">
+        <v>0.25</v>
+      </c>
+      <c r="L26" s="48">
+        <v>0.3</v>
+      </c>
+      <c r="M26" s="15">
+        <f t="shared" ref="M26" si="15">I26*K26*$D$8*100*100</f>
+        <v>1648.3249999999998</v>
+      </c>
+      <c r="N26" s="20">
+        <f t="shared" ref="N26" si="16">J26*L26*$D$8*100*100</f>
+        <v>1061.5500000000002</v>
+      </c>
+      <c r="O26" s="39">
+        <f t="shared" si="5"/>
+        <v>0.62066767779412424</v>
+      </c>
+      <c r="P26" s="41">
+        <f t="shared" si="6"/>
+        <v>0.96374362959822868</v>
+      </c>
+      <c r="Q26" s="12" t="str">
+        <f t="shared" si="7"/>
+        <v>WENO</v>
+      </c>
+      <c r="R26" t="s">
+        <v>12</v>
+      </c>
+      <c r="S26" s="27">
         <f t="shared" si="8"/>
-        <v>1037.1093999999998</v>
-      </c>
-      <c r="I26" s="34">
-        <f>AD25</f>
-        <v>94.19</v>
-      </c>
-      <c r="J26" s="35">
-        <f>AC25</f>
-        <v>50.55</v>
-      </c>
-      <c r="K26" s="57">
-        <v>0.25</v>
-      </c>
-      <c r="L26" s="60">
-        <v>0.3</v>
-      </c>
-      <c r="M26" s="34">
-        <f t="shared" ref="M26" si="13">I26*K26*$D$8*100*100</f>
-        <v>1648.3249999999998</v>
-      </c>
-      <c r="N26" s="35">
-        <f t="shared" ref="N26" si="14">J26*L26*$D$8*100*100</f>
-        <v>1061.5500000000002</v>
-      </c>
-      <c r="O26" s="31" t="str">
-        <f t="shared" si="5"/>
-        <v>WENO</v>
-      </c>
-      <c r="P26" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q26" s="43">
-        <f t="shared" si="6"/>
-        <v>611.21559999999999</v>
-      </c>
-      <c r="R26" s="44">
-        <f t="shared" si="7"/>
-        <v>24.440600000000359</v>
+        <v>625.26295000000005</v>
+      </c>
+      <c r="T26" s="28">
+        <f t="shared" si="9"/>
+        <v>38.48795000000041</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.3">
       <c r="G28" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="Q3:R26">
+  <conditionalFormatting sqref="S3:T26">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Mejora largos de los muros
</commit_message>
<xml_diff>
--- a/Tarea 02/Largos-muros.xlsx
+++ b/Tarea 02/Largos-muros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Google Drive\Trabajos\Proyecto de Hormigón Armado\proyecto-CI5206\Tarea 02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0C877A02-F512-4A82-BED8-370E12ED8C98}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A0DC7011-F304-4E62-979E-24A3A968D7C7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{02DCFF44-6514-457A-8521-53C0490CA4AF}"/>
   </bookViews>
@@ -153,9 +153,6 @@
     <t>piso tipo</t>
   </si>
   <si>
-    <t>Estac</t>
-  </si>
-  <si>
     <t>tipo piso</t>
   </si>
   <si>
@@ -172,14 +169,16 @@
   </si>
   <si>
     <t>% TauY</t>
+  </si>
+  <si>
+    <t>Estac (medio)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+  <numFmts count="1">
     <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
@@ -622,9 +621,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -634,10 +630,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -969,7 +968,7 @@
   <dimension ref="A1:AF28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P1" sqref="M1:P12"/>
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1028,10 +1027,10 @@
         <v>19</v>
       </c>
       <c r="O2" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="P2" s="9" t="s">
         <v>47</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>48</v>
       </c>
       <c r="Q2" s="9" t="s">
         <v>33</v>
@@ -1086,14 +1085,14 @@
         <v>1</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="52">
+      <c r="F3" s="51">
         <v>23</v>
       </c>
       <c r="G3" s="49">
         <f>$D$2*$D$4*$D$5</f>
         <v>41.04</v>
       </c>
-      <c r="H3" s="53">
+      <c r="H3" s="52">
         <f>G3</f>
         <v>41.04</v>
       </c>
@@ -1169,14 +1168,14 @@
         <v>1</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="52">
+      <c r="F4" s="51">
         <v>22</v>
       </c>
       <c r="G4" s="49">
         <f t="shared" ref="G4:G24" si="1">$D$2*$D$4*$D$5</f>
         <v>41.04</v>
       </c>
-      <c r="H4" s="53">
+      <c r="H4" s="52">
         <f>H3+G4</f>
         <v>82.08</v>
       </c>
@@ -1250,14 +1249,14 @@
         <v>0.1</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="52">
+      <c r="F5" s="51">
         <v>21</v>
       </c>
       <c r="G5" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H5" s="53">
+      <c r="H5" s="52">
         <f t="shared" ref="H5:H26" si="10">H4+G5</f>
         <v>123.12</v>
       </c>
@@ -1329,14 +1328,14 @@
         <v>7</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="52">
+      <c r="F6" s="51">
         <v>20</v>
       </c>
       <c r="G6" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H6" s="53">
+      <c r="H6" s="52">
         <f t="shared" si="10"/>
         <v>164.16</v>
       </c>
@@ -1402,14 +1401,14 @@
       <c r="AF6" s="11"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="F7" s="52">
+      <c r="F7" s="51">
         <v>19</v>
       </c>
       <c r="G7" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H7" s="53">
+      <c r="H7" s="52">
         <f t="shared" si="10"/>
         <v>205.2</v>
       </c>
@@ -1486,14 +1485,14 @@
         <f>D6/1000</f>
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="F8" s="52">
+      <c r="F8" s="51">
         <v>18</v>
       </c>
       <c r="G8" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H8" s="53">
+      <c r="H8" s="52">
         <f t="shared" si="10"/>
         <v>246.23999999999998</v>
       </c>
@@ -1563,14 +1562,14 @@
       <c r="B9" s="37"/>
       <c r="C9" s="4"/>
       <c r="D9" s="5"/>
-      <c r="F9" s="52">
+      <c r="F9" s="51">
         <v>17</v>
       </c>
       <c r="G9" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H9" s="53">
+      <c r="H9" s="52">
         <f t="shared" si="10"/>
         <v>287.27999999999997</v>
       </c>
@@ -1638,14 +1637,14 @@
       <c r="B10" s="37"/>
       <c r="C10" s="4"/>
       <c r="D10" s="5"/>
-      <c r="F10" s="52">
+      <c r="F10" s="51">
         <v>16</v>
       </c>
       <c r="G10" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H10" s="53">
+      <c r="H10" s="52">
         <f t="shared" si="10"/>
         <v>328.32</v>
       </c>
@@ -1722,14 +1721,14 @@
         <f>D2</f>
         <v>410.4</v>
       </c>
-      <c r="F11" s="52">
+      <c r="F11" s="51">
         <v>15</v>
       </c>
       <c r="G11" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H11" s="53">
+      <c r="H11" s="52">
         <f t="shared" si="10"/>
         <v>369.36</v>
       </c>
@@ -1801,14 +1800,14 @@
       <c r="D12" s="6">
         <v>-55.494999999999997</v>
       </c>
-      <c r="F12" s="52">
+      <c r="F12" s="51">
         <v>14</v>
       </c>
       <c r="G12" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H12" s="53">
+      <c r="H12" s="52">
         <f t="shared" si="10"/>
         <v>410.40000000000003</v>
       </c>
@@ -1882,14 +1881,14 @@
       <c r="D13" s="6">
         <v>-28.218</v>
       </c>
-      <c r="F13" s="52">
+      <c r="F13" s="51">
         <v>13</v>
       </c>
       <c r="G13" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H13" s="53">
+      <c r="H13" s="52">
         <f t="shared" si="10"/>
         <v>451.44000000000005</v>
       </c>
@@ -1957,21 +1956,21 @@
     <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="34"/>
-      <c r="C14" s="4" t="s">
-        <v>42</v>
+      <c r="C14" s="37" t="s">
+        <v>48</v>
       </c>
       <c r="D14" s="6">
         <f>280.947/2</f>
         <v>140.4735</v>
       </c>
-      <c r="F14" s="52">
+      <c r="F14" s="51">
         <v>12</v>
       </c>
       <c r="G14" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H14" s="53">
+      <c r="H14" s="52">
         <f t="shared" si="10"/>
         <v>492.48000000000008</v>
       </c>
@@ -2039,14 +2038,14 @@
       <c r="B15" s="34"/>
       <c r="C15" s="4"/>
       <c r="D15" s="6"/>
-      <c r="F15" s="52">
+      <c r="F15" s="51">
         <v>11</v>
       </c>
       <c r="G15" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H15" s="53">
+      <c r="H15" s="52">
         <f t="shared" si="10"/>
         <v>533.5200000000001</v>
       </c>
@@ -2116,14 +2115,14 @@
       <c r="B16" s="34"/>
       <c r="C16" s="4"/>
       <c r="D16" s="6"/>
-      <c r="F16" s="52">
+      <c r="F16" s="51">
         <v>10</v>
       </c>
       <c r="G16" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H16" s="53">
+      <c r="H16" s="52">
         <f t="shared" si="10"/>
         <v>574.56000000000006</v>
       </c>
@@ -2191,14 +2190,14 @@
       <c r="B17" s="34"/>
       <c r="C17" s="4"/>
       <c r="D17" s="6"/>
-      <c r="F17" s="52">
+      <c r="F17" s="51">
         <v>9</v>
       </c>
       <c r="G17" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H17" s="53">
+      <c r="H17" s="52">
         <f t="shared" si="10"/>
         <v>615.6</v>
       </c>
@@ -2271,14 +2270,14 @@
         <f>SUM(D11:D14)</f>
         <v>467.16049999999996</v>
       </c>
-      <c r="F18" s="52">
+      <c r="F18" s="51">
         <v>8</v>
       </c>
       <c r="G18" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H18" s="53">
+      <c r="H18" s="52">
         <f t="shared" si="10"/>
         <v>656.64</v>
       </c>
@@ -2342,14 +2341,14 @@
       <c r="B19" s="37"/>
       <c r="C19" s="4"/>
       <c r="D19" s="5"/>
-      <c r="F19" s="52">
+      <c r="F19" s="51">
         <v>7</v>
       </c>
       <c r="G19" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H19" s="53">
+      <c r="H19" s="52">
         <f t="shared" si="10"/>
         <v>697.68</v>
       </c>
@@ -2416,19 +2415,19 @@
         <v>40</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D20" s="4">
         <v>1066.5999999999999</v>
       </c>
-      <c r="F20" s="52">
+      <c r="F20" s="51">
         <v>6</v>
       </c>
       <c r="G20" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H20" s="53">
+      <c r="H20" s="52">
         <f t="shared" si="10"/>
         <v>738.71999999999991</v>
       </c>
@@ -2491,20 +2490,20 @@
       <c r="A21" s="5"/>
       <c r="B21" s="37"/>
       <c r="C21" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21" s="5">
         <f>-7.68</f>
         <v>-7.68</v>
       </c>
-      <c r="F21" s="52">
+      <c r="F21" s="51">
         <v>5</v>
       </c>
       <c r="G21" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H21" s="53">
+      <c r="H21" s="52">
         <f t="shared" si="10"/>
         <v>779.75999999999988</v>
       </c>
@@ -2565,20 +2564,20 @@
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.3">
       <c r="C22" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D22">
         <f>D20+D21</f>
         <v>1058.9199999999998</v>
       </c>
-      <c r="F22" s="52">
+      <c r="F22" s="51">
         <v>4</v>
       </c>
       <c r="G22" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H22" s="53">
+      <c r="H22" s="52">
         <f t="shared" si="10"/>
         <v>820.79999999999984</v>
       </c>
@@ -2638,14 +2637,14 @@
       <c r="AF22" s="11"/>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="F23" s="52">
+      <c r="F23" s="51">
         <v>3</v>
       </c>
       <c r="G23" s="49">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H23" s="53">
+      <c r="H23" s="52">
         <f t="shared" si="10"/>
         <v>861.8399999999998</v>
       </c>
@@ -2704,7 +2703,7 @@
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.3">
       <c r="C24" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D24">
         <f>(D22-D2)/2+D2</f>
@@ -2713,14 +2712,14 @@
       <c r="E24" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="52">
+      <c r="F24" s="51">
         <v>2</v>
       </c>
       <c r="G24" s="50">
         <f t="shared" si="1"/>
         <v>41.04</v>
       </c>
-      <c r="H24" s="53">
+      <c r="H24" s="52">
         <f t="shared" si="10"/>
         <v>902.87999999999977</v>
       </c>
@@ -2781,14 +2780,14 @@
       <c r="E25" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="52">
+      <c r="F25" s="51">
         <v>1</v>
       </c>
-      <c r="G25" s="51">
+      <c r="G25" s="50">
         <f>$D$18*$D$4*$D$5</f>
         <v>46.716049999999996</v>
       </c>
-      <c r="H25" s="53">
+      <c r="H25" s="54">
         <f t="shared" si="10"/>
         <v>949.59604999999976</v>
       </c>
@@ -2875,14 +2874,14 @@
       <c r="E26" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="54">
+      <c r="F26" s="53">
         <v>-1</v>
       </c>
-      <c r="G26" s="55">
+      <c r="G26" s="56">
         <f>$D$24*$D$4*$D$5</f>
         <v>73.465999999999994</v>
       </c>
-      <c r="H26" s="56">
+      <c r="H26" s="55">
         <f t="shared" si="10"/>
         <v>1023.0620499999998</v>
       </c>

</xml_diff>

<commit_message>
cambio espesor de muros para uniformizar 3, 4 y 5
</commit_message>
<xml_diff>
--- a/Tarea 02/Largos-muros.xlsx
+++ b/Tarea 02/Largos-muros.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Google Drive\Trabajos\Proyecto de Hormigón Armado\proyecto-CI5206\Tarea 02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ramos Ingenieria\12° Semestre\Proyecto de Hormigón Armado\Tarea 02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A0DC7011-F304-4E62-979E-24A3A968D7C7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA001CC8-1205-4B1E-BD82-5B750E55F897}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{02DCFF44-6514-457A-8521-53C0490CA4AF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5655" xr2:uid="{02DCFF44-6514-457A-8521-53C0490CA4AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -179,7 +179,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -205,7 +205,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,6 +230,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -477,7 +483,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -582,16 +588,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -637,12 +643,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -669,7 +678,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -967,29 +976,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86364C21-7A4B-487E-B815-3438660120DA}">
   <dimension ref="A1:AF28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" topLeftCell="D14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.33203125" customWidth="1"/>
-    <col min="12" max="12" width="7.5546875" customWidth="1"/>
-    <col min="13" max="13" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="8.44140625" customWidth="1"/>
-    <col min="18" max="18" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="23" max="31" width="11.5546875" style="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.28515625" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="8.42578125" customWidth="1"/>
+    <col min="18" max="18" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="31" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
@@ -1074,7 +1083,7 @@
         <v>-1 X</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1098,7 +1107,7 @@
       </c>
       <c r="I3" s="18">
         <f>$X$25</f>
-        <v>61.86</v>
+        <v>58.02</v>
       </c>
       <c r="J3" s="14">
         <f>$W$25</f>
@@ -1112,7 +1121,7 @@
       </c>
       <c r="M3" s="13">
         <f t="shared" ref="M3:M22" si="0">I3*K3*$D$8*100*100</f>
-        <v>866.04</v>
+        <v>812.2800000000002</v>
       </c>
       <c r="N3" s="18">
         <f>J3*L3*$D$8*100*100</f>
@@ -1120,7 +1129,7 @@
       </c>
       <c r="O3" s="38">
         <f>H3/M3</f>
-        <v>4.738811140363032E-2</v>
+        <v>5.0524449697148754E-2</v>
       </c>
       <c r="P3" s="40">
         <f>H3/N3</f>
@@ -1132,7 +1141,7 @@
       </c>
       <c r="S3" s="23">
         <f>M3-H3</f>
-        <v>825</v>
+        <v>771.24000000000024</v>
       </c>
       <c r="T3" s="24">
         <f>N3-H3</f>
@@ -1157,7 +1166,7 @@
       <c r="AE3" s="10"/>
       <c r="AF3" s="11"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1181,7 +1190,7 @@
       </c>
       <c r="I4" s="18">
         <f t="shared" ref="I4:I22" si="2">$X$25</f>
-        <v>61.86</v>
+        <v>58.02</v>
       </c>
       <c r="J4" s="14">
         <f t="shared" ref="J4:J22" si="3">$W$25</f>
@@ -1195,7 +1204,7 @@
       </c>
       <c r="M4" s="13">
         <f t="shared" si="0"/>
-        <v>866.04</v>
+        <v>812.2800000000002</v>
       </c>
       <c r="N4" s="18">
         <f t="shared" ref="N4:N22" si="4">J4*L4*$D$8*100*100</f>
@@ -1203,7 +1212,7 @@
       </c>
       <c r="O4" s="38">
         <f t="shared" ref="O4:O26" si="5">H4/M4</f>
-        <v>9.4776222807260641E-2</v>
+        <v>0.10104889939429751</v>
       </c>
       <c r="P4" s="40">
         <f t="shared" ref="P4:P26" si="6">H4/N4</f>
@@ -1215,7 +1224,7 @@
       </c>
       <c r="S4" s="25">
         <f t="shared" ref="S4:S26" si="8">M4-H4</f>
-        <v>783.95999999999992</v>
+        <v>730.20000000000016</v>
       </c>
       <c r="T4" s="26">
         <f t="shared" ref="T4:T26" si="9">N4-H4</f>
@@ -1238,7 +1247,7 @@
       <c r="AE4" s="10"/>
       <c r="AF4" s="11"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1262,7 +1271,7 @@
       </c>
       <c r="I5" s="18">
         <f t="shared" si="2"/>
-        <v>61.86</v>
+        <v>58.02</v>
       </c>
       <c r="J5" s="14">
         <f t="shared" si="3"/>
@@ -1276,7 +1285,7 @@
       </c>
       <c r="M5" s="13">
         <f t="shared" si="0"/>
-        <v>866.04</v>
+        <v>812.2800000000002</v>
       </c>
       <c r="N5" s="18">
         <f t="shared" si="4"/>
@@ -1284,7 +1293,7 @@
       </c>
       <c r="O5" s="38">
         <f t="shared" si="5"/>
-        <v>0.14216433421089097</v>
+        <v>0.15157334909144626</v>
       </c>
       <c r="P5" s="40">
         <f t="shared" si="6"/>
@@ -1296,7 +1305,7 @@
       </c>
       <c r="S5" s="25">
         <f t="shared" si="8"/>
-        <v>742.92</v>
+        <v>689.1600000000002</v>
       </c>
       <c r="T5" s="26">
         <f t="shared" si="9"/>
@@ -1317,7 +1326,7 @@
       <c r="AE5" s="10"/>
       <c r="AF5" s="11"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
@@ -1341,7 +1350,7 @@
       </c>
       <c r="I6" s="18">
         <f t="shared" si="2"/>
-        <v>61.86</v>
+        <v>58.02</v>
       </c>
       <c r="J6" s="14">
         <f t="shared" si="3"/>
@@ -1355,7 +1364,7 @@
       </c>
       <c r="M6" s="13">
         <f t="shared" si="0"/>
-        <v>866.04</v>
+        <v>812.2800000000002</v>
       </c>
       <c r="N6" s="18">
         <f t="shared" si="4"/>
@@ -1363,7 +1372,7 @@
       </c>
       <c r="O6" s="38">
         <f t="shared" si="5"/>
-        <v>0.18955244561452128</v>
+        <v>0.20209779878859502</v>
       </c>
       <c r="P6" s="40">
         <f t="shared" si="6"/>
@@ -1375,7 +1384,7 @@
       </c>
       <c r="S6" s="25">
         <f t="shared" si="8"/>
-        <v>701.88</v>
+        <v>648.12000000000023</v>
       </c>
       <c r="T6" s="26">
         <f t="shared" si="9"/>
@@ -1400,7 +1409,7 @@
       <c r="AE6" s="10"/>
       <c r="AF6" s="11"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="F7" s="51">
         <v>19</v>
       </c>
@@ -1414,7 +1423,7 @@
       </c>
       <c r="I7" s="18">
         <f t="shared" si="2"/>
-        <v>61.86</v>
+        <v>58.02</v>
       </c>
       <c r="J7" s="14">
         <f t="shared" si="3"/>
@@ -1428,7 +1437,7 @@
       </c>
       <c r="M7" s="13">
         <f t="shared" si="0"/>
-        <v>866.04</v>
+        <v>812.2800000000002</v>
       </c>
       <c r="N7" s="18">
         <f t="shared" si="4"/>
@@ -1436,7 +1445,7 @@
       </c>
       <c r="O7" s="38">
         <f t="shared" si="5"/>
-        <v>0.23694055701815159</v>
+        <v>0.25262224848574377</v>
       </c>
       <c r="P7" s="40">
         <f t="shared" si="6"/>
@@ -1448,7 +1457,7 @@
       </c>
       <c r="S7" s="25">
         <f t="shared" si="8"/>
-        <v>660.83999999999992</v>
+        <v>607.08000000000015</v>
       </c>
       <c r="T7" s="26">
         <f t="shared" si="9"/>
@@ -1473,7 +1482,7 @@
       <c r="AE7" s="10"/>
       <c r="AF7" s="11"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="37" t="s">
         <v>20</v>
@@ -1498,7 +1507,7 @@
       </c>
       <c r="I8" s="18">
         <f t="shared" si="2"/>
-        <v>61.86</v>
+        <v>58.02</v>
       </c>
       <c r="J8" s="14">
         <f t="shared" si="3"/>
@@ -1512,7 +1521,7 @@
       </c>
       <c r="M8" s="13">
         <f t="shared" si="0"/>
-        <v>866.04</v>
+        <v>812.2800000000002</v>
       </c>
       <c r="N8" s="18">
         <f t="shared" si="4"/>
@@ -1520,7 +1529,7 @@
       </c>
       <c r="O8" s="38">
         <f t="shared" si="5"/>
-        <v>0.28432866842178189</v>
+        <v>0.30314669818289253</v>
       </c>
       <c r="P8" s="40">
         <f t="shared" si="6"/>
@@ -1532,7 +1541,7 @@
       </c>
       <c r="S8" s="25">
         <f t="shared" si="8"/>
-        <v>619.79999999999995</v>
+        <v>566.04000000000019</v>
       </c>
       <c r="T8" s="26">
         <f t="shared" si="9"/>
@@ -1557,7 +1566,7 @@
       <c r="AE8" s="10"/>
       <c r="AF8" s="11"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="37"/>
       <c r="C9" s="4"/>
@@ -1575,7 +1584,7 @@
       </c>
       <c r="I9" s="18">
         <f t="shared" si="2"/>
-        <v>61.86</v>
+        <v>58.02</v>
       </c>
       <c r="J9" s="14">
         <f t="shared" si="3"/>
@@ -1589,7 +1598,7 @@
       </c>
       <c r="M9" s="13">
         <f t="shared" si="0"/>
-        <v>866.04</v>
+        <v>812.2800000000002</v>
       </c>
       <c r="N9" s="18">
         <f t="shared" si="4"/>
@@ -1597,7 +1606,7 @@
       </c>
       <c r="O9" s="38">
         <f t="shared" si="5"/>
-        <v>0.3317167798254122</v>
+        <v>0.35367114788004123</v>
       </c>
       <c r="P9" s="40">
         <f t="shared" si="6"/>
@@ -1609,7 +1618,7 @@
       </c>
       <c r="S9" s="25">
         <f t="shared" si="8"/>
-        <v>578.76</v>
+        <v>525.00000000000023</v>
       </c>
       <c r="T9" s="26">
         <f t="shared" si="9"/>
@@ -1632,7 +1641,7 @@
       <c r="AE9" s="10"/>
       <c r="AF9" s="11"/>
     </row>
-    <row r="10" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="37"/>
       <c r="C10" s="4"/>
@@ -1650,7 +1659,7 @@
       </c>
       <c r="I10" s="18">
         <f t="shared" si="2"/>
-        <v>61.86</v>
+        <v>58.02</v>
       </c>
       <c r="J10" s="14">
         <f t="shared" si="3"/>
@@ -1664,7 +1673,7 @@
       </c>
       <c r="M10" s="13">
         <f t="shared" si="0"/>
-        <v>866.04</v>
+        <v>812.2800000000002</v>
       </c>
       <c r="N10" s="18">
         <f t="shared" si="4"/>
@@ -1672,7 +1681,7 @@
       </c>
       <c r="O10" s="38">
         <f t="shared" si="5"/>
-        <v>0.37910489122904256</v>
+        <v>0.40419559757719004</v>
       </c>
       <c r="P10" s="40">
         <f t="shared" si="6"/>
@@ -1684,7 +1693,7 @@
       </c>
       <c r="S10" s="25">
         <f t="shared" si="8"/>
-        <v>537.72</v>
+        <v>483.96000000000021</v>
       </c>
       <c r="T10" s="26">
         <f t="shared" si="9"/>
@@ -1709,7 +1718,7 @@
       <c r="AE10" s="10"/>
       <c r="AF10" s="11"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="32" t="s">
         <v>36</v>
@@ -1734,7 +1743,7 @@
       </c>
       <c r="I11" s="18">
         <f t="shared" si="2"/>
-        <v>61.86</v>
+        <v>58.02</v>
       </c>
       <c r="J11" s="14">
         <f t="shared" si="3"/>
@@ -1748,7 +1757,7 @@
       </c>
       <c r="M11" s="13">
         <f t="shared" si="0"/>
-        <v>866.04</v>
+        <v>812.2800000000002</v>
       </c>
       <c r="N11" s="18">
         <f t="shared" si="4"/>
@@ -1756,7 +1765,7 @@
       </c>
       <c r="O11" s="38">
         <f t="shared" si="5"/>
-        <v>0.42649300263267287</v>
+        <v>0.45472004727433879</v>
       </c>
       <c r="P11" s="40">
         <f t="shared" si="6"/>
@@ -1768,7 +1777,7 @@
       </c>
       <c r="S11" s="25">
         <f t="shared" si="8"/>
-        <v>496.67999999999995</v>
+        <v>442.92000000000019</v>
       </c>
       <c r="T11" s="26">
         <f t="shared" si="9"/>
@@ -1791,7 +1800,7 @@
       <c r="AE11" s="10"/>
       <c r="AF11" s="11"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="34"/>
       <c r="C12" s="4" t="s">
@@ -1813,7 +1822,7 @@
       </c>
       <c r="I12" s="18">
         <f t="shared" si="2"/>
-        <v>61.86</v>
+        <v>58.02</v>
       </c>
       <c r="J12" s="14">
         <f t="shared" si="3"/>
@@ -1827,7 +1836,7 @@
       </c>
       <c r="M12" s="13">
         <f t="shared" si="0"/>
-        <v>866.04</v>
+        <v>812.2800000000002</v>
       </c>
       <c r="N12" s="18">
         <f t="shared" si="4"/>
@@ -1835,7 +1844,7 @@
       </c>
       <c r="O12" s="38">
         <f t="shared" si="5"/>
-        <v>0.47388111403630323</v>
+        <v>0.50524449697148754</v>
       </c>
       <c r="P12" s="40">
         <f t="shared" si="6"/>
@@ -1847,7 +1856,7 @@
       </c>
       <c r="S12" s="25">
         <f t="shared" si="8"/>
-        <v>455.63999999999993</v>
+        <v>401.88000000000017</v>
       </c>
       <c r="T12" s="26">
         <f t="shared" si="9"/>
@@ -1872,7 +1881,7 @@
       <c r="AE12" s="10"/>
       <c r="AF12" s="11"/>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="34"/>
       <c r="C13" s="4" t="s">
@@ -1894,7 +1903,7 @@
       </c>
       <c r="I13" s="18">
         <f t="shared" si="2"/>
-        <v>61.86</v>
+        <v>58.02</v>
       </c>
       <c r="J13" s="14">
         <f t="shared" si="3"/>
@@ -1908,7 +1917,7 @@
       </c>
       <c r="M13" s="13">
         <f t="shared" si="0"/>
-        <v>866.04</v>
+        <v>812.2800000000002</v>
       </c>
       <c r="N13" s="18">
         <f t="shared" si="4"/>
@@ -1916,7 +1925,7 @@
       </c>
       <c r="O13" s="38">
         <f t="shared" si="5"/>
-        <v>0.52126922543993359</v>
+        <v>0.55576894666863641</v>
       </c>
       <c r="P13" s="40">
         <f t="shared" si="6"/>
@@ -1928,7 +1937,7 @@
       </c>
       <c r="S13" s="25">
         <f t="shared" si="8"/>
-        <v>414.59999999999991</v>
+        <v>360.84000000000015</v>
       </c>
       <c r="T13" s="26">
         <f t="shared" si="9"/>
@@ -1953,7 +1962,7 @@
       <c r="AE13" s="10"/>
       <c r="AF13" s="11"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="34"/>
       <c r="C14" s="37" t="s">
@@ -1976,7 +1985,7 @@
       </c>
       <c r="I14" s="18">
         <f t="shared" si="2"/>
-        <v>61.86</v>
+        <v>58.02</v>
       </c>
       <c r="J14" s="14">
         <f t="shared" si="3"/>
@@ -1990,7 +1999,7 @@
       </c>
       <c r="M14" s="13">
         <f t="shared" si="0"/>
-        <v>866.04</v>
+        <v>812.2800000000002</v>
       </c>
       <c r="N14" s="18">
         <f t="shared" si="4"/>
@@ -1998,7 +2007,7 @@
       </c>
       <c r="O14" s="38">
         <f t="shared" si="5"/>
-        <v>0.5686573368435639</v>
+        <v>0.60629339636578516</v>
       </c>
       <c r="P14" s="40">
         <f t="shared" si="6"/>
@@ -2010,7 +2019,7 @@
       </c>
       <c r="S14" s="25">
         <f t="shared" si="8"/>
-        <v>373.55999999999989</v>
+        <v>319.80000000000013</v>
       </c>
       <c r="T14" s="26">
         <f t="shared" si="9"/>
@@ -2033,7 +2042,7 @@
       <c r="AE14" s="10"/>
       <c r="AF14" s="11"/>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="34"/>
       <c r="C15" s="4"/>
@@ -2051,7 +2060,7 @@
       </c>
       <c r="I15" s="18">
         <f t="shared" si="2"/>
-        <v>61.86</v>
+        <v>58.02</v>
       </c>
       <c r="J15" s="14">
         <f t="shared" si="3"/>
@@ -2065,7 +2074,7 @@
       </c>
       <c r="M15" s="13">
         <f t="shared" si="0"/>
-        <v>866.04</v>
+        <v>812.2800000000002</v>
       </c>
       <c r="N15" s="18">
         <f t="shared" si="4"/>
@@ -2073,7 +2082,7 @@
       </c>
       <c r="O15" s="38">
         <f t="shared" si="5"/>
-        <v>0.61604544824719432</v>
+        <v>0.65681784606293392</v>
       </c>
       <c r="P15" s="40">
         <f t="shared" si="6"/>
@@ -2085,7 +2094,7 @@
       </c>
       <c r="S15" s="25">
         <f t="shared" si="8"/>
-        <v>332.51999999999987</v>
+        <v>278.7600000000001</v>
       </c>
       <c r="T15" s="26">
         <f t="shared" si="9"/>
@@ -2110,7 +2119,7 @@
       <c r="AE15" s="10"/>
       <c r="AF15" s="11"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="34"/>
       <c r="C16" s="4"/>
@@ -2128,7 +2137,7 @@
       </c>
       <c r="I16" s="18">
         <f t="shared" si="2"/>
-        <v>61.86</v>
+        <v>58.02</v>
       </c>
       <c r="J16" s="14">
         <f t="shared" si="3"/>
@@ -2142,7 +2151,7 @@
       </c>
       <c r="M16" s="13">
         <f t="shared" si="0"/>
-        <v>866.04</v>
+        <v>812.2800000000002</v>
       </c>
       <c r="N16" s="18">
         <f t="shared" si="4"/>
@@ -2150,7 +2159,7 @@
       </c>
       <c r="O16" s="38">
         <f t="shared" si="5"/>
-        <v>0.66343355965082451</v>
+        <v>0.70734229576008267</v>
       </c>
       <c r="P16" s="40">
         <f t="shared" si="6"/>
@@ -2162,7 +2171,7 @@
       </c>
       <c r="S16" s="25">
         <f t="shared" si="8"/>
-        <v>291.4799999999999</v>
+        <v>237.72000000000014</v>
       </c>
       <c r="T16" s="26">
         <f t="shared" si="9"/>
@@ -2185,7 +2194,7 @@
       <c r="AE16" s="10"/>
       <c r="AF16" s="11"/>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="34"/>
       <c r="C17" s="4"/>
@@ -2203,7 +2212,7 @@
       </c>
       <c r="I17" s="18">
         <f t="shared" si="2"/>
-        <v>61.86</v>
+        <v>58.02</v>
       </c>
       <c r="J17" s="14">
         <f t="shared" si="3"/>
@@ -2217,7 +2226,7 @@
       </c>
       <c r="M17" s="13">
         <f t="shared" si="0"/>
-        <v>866.04</v>
+        <v>812.2800000000002</v>
       </c>
       <c r="N17" s="18">
         <f t="shared" si="4"/>
@@ -2225,7 +2234,7 @@
       </c>
       <c r="O17" s="38">
         <f t="shared" si="5"/>
-        <v>0.71082167105445482</v>
+        <v>0.75786674545723132</v>
       </c>
       <c r="P17" s="40">
         <f t="shared" si="6"/>
@@ -2237,7 +2246,7 @@
       </c>
       <c r="S17" s="25">
         <f t="shared" si="8"/>
-        <v>250.43999999999994</v>
+        <v>196.68000000000018</v>
       </c>
       <c r="T17" s="26">
         <f t="shared" si="9"/>
@@ -2260,7 +2269,7 @@
       <c r="AE17" s="10"/>
       <c r="AF17" s="11"/>
     </row>
-    <row r="18" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36" t="s">
@@ -2283,7 +2292,7 @@
       </c>
       <c r="I18" s="18">
         <f t="shared" si="2"/>
-        <v>61.86</v>
+        <v>58.02</v>
       </c>
       <c r="J18" s="14">
         <f t="shared" si="3"/>
@@ -2297,7 +2306,7 @@
       </c>
       <c r="M18" s="13">
         <f t="shared" si="0"/>
-        <v>866.04</v>
+        <v>812.2800000000002</v>
       </c>
       <c r="N18" s="18">
         <f t="shared" si="4"/>
@@ -2305,7 +2314,7 @@
       </c>
       <c r="O18" s="38">
         <f t="shared" si="5"/>
-        <v>0.75820978245808512</v>
+        <v>0.80839119515438007</v>
       </c>
       <c r="P18" s="40">
         <f t="shared" si="6"/>
@@ -2317,7 +2326,7 @@
       </c>
       <c r="S18" s="25">
         <f t="shared" si="8"/>
-        <v>209.39999999999998</v>
+        <v>155.64000000000021</v>
       </c>
       <c r="T18" s="26">
         <f t="shared" si="9"/>
@@ -2336,7 +2345,7 @@
       <c r="AE18" s="10"/>
       <c r="AF18" s="11"/>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="37"/>
       <c r="C19" s="4"/>
@@ -2354,7 +2363,7 @@
       </c>
       <c r="I19" s="18">
         <f t="shared" si="2"/>
-        <v>61.86</v>
+        <v>58.02</v>
       </c>
       <c r="J19" s="14">
         <f t="shared" si="3"/>
@@ -2368,7 +2377,7 @@
       </c>
       <c r="M19" s="13">
         <f t="shared" si="0"/>
-        <v>866.04</v>
+        <v>812.2800000000002</v>
       </c>
       <c r="N19" s="18">
         <f t="shared" si="4"/>
@@ -2376,7 +2385,7 @@
       </c>
       <c r="O19" s="38">
         <f t="shared" si="5"/>
-        <v>0.80559789386171532</v>
+        <v>0.85891564485152871</v>
       </c>
       <c r="P19" s="40">
         <f t="shared" si="6"/>
@@ -2388,7 +2397,7 @@
       </c>
       <c r="S19" s="25">
         <f t="shared" si="8"/>
-        <v>168.36</v>
+        <v>114.60000000000025</v>
       </c>
       <c r="T19" s="26">
         <f t="shared" si="9"/>
@@ -2409,7 +2418,7 @@
       <c r="AE19" s="10"/>
       <c r="AF19" s="11"/>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="37" t="s">
         <v>40</v>
@@ -2433,7 +2442,7 @@
       </c>
       <c r="I20" s="18">
         <f t="shared" si="2"/>
-        <v>61.86</v>
+        <v>58.02</v>
       </c>
       <c r="J20" s="14">
         <f t="shared" si="3"/>
@@ -2447,7 +2456,7 @@
       </c>
       <c r="M20" s="13">
         <f t="shared" si="0"/>
-        <v>866.04</v>
+        <v>812.2800000000002</v>
       </c>
       <c r="N20" s="18">
         <f t="shared" si="4"/>
@@ -2455,7 +2464,7 @@
       </c>
       <c r="O20" s="38">
         <f t="shared" si="5"/>
-        <v>0.85298600526534563</v>
+        <v>0.90944009454867747</v>
       </c>
       <c r="P20" s="40">
         <f t="shared" si="6"/>
@@ -2467,7 +2476,7 @@
       </c>
       <c r="S20" s="25">
         <f t="shared" si="8"/>
-        <v>127.32000000000005</v>
+        <v>73.560000000000286</v>
       </c>
       <c r="T20" s="26">
         <f t="shared" si="9"/>
@@ -2476,7 +2485,9 @@
       <c r="W20" s="10">
         <v>5.5</v>
       </c>
-      <c r="X20" s="11"/>
+      <c r="X20" s="11">
+        <v>-1.92</v>
+      </c>
       <c r="Y20" s="10"/>
       <c r="Z20" s="11"/>
       <c r="AA20" s="10"/>
@@ -2486,7 +2497,7 @@
       <c r="AE20" s="10"/>
       <c r="AF20" s="11"/>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="37"/>
       <c r="C21" s="4" t="s">
@@ -2509,21 +2520,21 @@
       </c>
       <c r="I21" s="18">
         <f t="shared" si="2"/>
-        <v>61.86</v>
+        <v>58.02</v>
       </c>
       <c r="J21" s="14">
         <f t="shared" si="3"/>
         <v>53.12</v>
       </c>
-      <c r="K21" s="44">
-        <v>0.2</v>
+      <c r="K21" s="57">
+        <v>0.25</v>
       </c>
       <c r="L21" s="43">
         <v>0.25</v>
       </c>
       <c r="M21" s="13">
         <f t="shared" si="0"/>
-        <v>866.04</v>
+        <v>1015.3500000000001</v>
       </c>
       <c r="N21" s="18">
         <f t="shared" si="4"/>
@@ -2531,7 +2542,7 @@
       </c>
       <c r="O21" s="38">
         <f t="shared" si="5"/>
-        <v>0.90037411666897593</v>
+        <v>0.76797163539666102</v>
       </c>
       <c r="P21" s="40">
         <f t="shared" si="6"/>
@@ -2543,7 +2554,7 @@
       </c>
       <c r="S21" s="25">
         <f t="shared" si="8"/>
-        <v>86.280000000000086</v>
+        <v>235.59000000000026</v>
       </c>
       <c r="T21" s="26">
         <f t="shared" si="9"/>
@@ -2552,7 +2563,9 @@
       <c r="W21" s="10">
         <v>3.08</v>
       </c>
-      <c r="X21" s="11"/>
+      <c r="X21" s="11">
+        <v>-1.92</v>
+      </c>
       <c r="Y21" s="10"/>
       <c r="Z21" s="11"/>
       <c r="AA21" s="10"/>
@@ -2562,7 +2575,7 @@
       <c r="AE21" s="10"/>
       <c r="AF21" s="11"/>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>44</v>
       </c>
@@ -2583,21 +2596,21 @@
       </c>
       <c r="I22" s="18">
         <f t="shared" si="2"/>
-        <v>61.86</v>
+        <v>58.02</v>
       </c>
       <c r="J22" s="14">
         <f t="shared" si="3"/>
         <v>53.12</v>
       </c>
-      <c r="K22" s="44">
-        <v>0.2</v>
+      <c r="K22" s="57">
+        <v>0.25</v>
       </c>
       <c r="L22" s="43">
         <v>0.25</v>
       </c>
       <c r="M22" s="13">
         <f t="shared" si="0"/>
-        <v>866.04</v>
+        <v>1015.3500000000001</v>
       </c>
       <c r="N22" s="18">
         <f t="shared" si="4"/>
@@ -2605,7 +2618,7 @@
       </c>
       <c r="O22" s="38">
         <f t="shared" si="5"/>
-        <v>0.94776222807260624</v>
+        <v>0.80839119515437996</v>
       </c>
       <c r="P22" s="40">
         <f t="shared" si="6"/>
@@ -2617,7 +2630,7 @@
       </c>
       <c r="S22" s="25">
         <f t="shared" si="8"/>
-        <v>45.240000000000123</v>
+        <v>194.5500000000003</v>
       </c>
       <c r="T22" s="26">
         <f t="shared" si="9"/>
@@ -2636,7 +2649,7 @@
       <c r="AE22" s="10"/>
       <c r="AF22" s="11"/>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="F23" s="51">
         <v>3</v>
       </c>
@@ -2650,21 +2663,21 @@
       </c>
       <c r="I23" s="18">
         <f>Z25</f>
-        <v>61.86</v>
+        <v>58.02</v>
       </c>
       <c r="J23" s="14">
         <f>Y25</f>
         <v>50.03</v>
       </c>
-      <c r="K23" s="44">
-        <v>0.2</v>
+      <c r="K23" s="57">
+        <v>0.25</v>
       </c>
       <c r="L23" s="43">
         <v>0.25</v>
       </c>
       <c r="M23" s="13">
         <f t="shared" ref="M23:M24" si="11">I23*K23*$D$8*100*100</f>
-        <v>866.04</v>
+        <v>1015.3500000000001</v>
       </c>
       <c r="N23" s="18">
         <f t="shared" ref="N23:N24" si="12">J23*L23*$D$8*100*100</f>
@@ -2672,7 +2685,7 @@
       </c>
       <c r="O23" s="38">
         <f t="shared" si="5"/>
-        <v>0.99515033947623643</v>
+        <v>0.84881075491209901</v>
       </c>
       <c r="P23" s="40">
         <f t="shared" si="6"/>
@@ -2684,7 +2697,7 @@
       </c>
       <c r="S23" s="25">
         <f t="shared" si="8"/>
-        <v>4.2000000000001592</v>
+        <v>153.51000000000033</v>
       </c>
       <c r="T23" s="26">
         <f t="shared" si="9"/>
@@ -2701,7 +2714,7 @@
       <c r="AE23" s="10"/>
       <c r="AF23" s="11"/>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
         <v>45</v>
       </c>
@@ -2725,7 +2738,7 @@
       </c>
       <c r="I24" s="18">
         <f>AB25</f>
-        <v>60.38</v>
+        <v>57.05</v>
       </c>
       <c r="J24" s="14">
         <f>AA25</f>
@@ -2739,7 +2752,7 @@
       </c>
       <c r="M24" s="13">
         <f t="shared" si="11"/>
-        <v>1056.6500000000001</v>
+        <v>998.37499999999989</v>
       </c>
       <c r="N24" s="18">
         <f t="shared" si="12"/>
@@ -2747,7 +2760,7 @@
       </c>
       <c r="O24" s="38">
         <f t="shared" si="5"/>
-        <v>0.85447404533194504</v>
+        <v>0.90434956804807798</v>
       </c>
       <c r="P24" s="40">
         <f t="shared" si="6"/>
@@ -2759,7 +2772,7 @@
       </c>
       <c r="S24" s="25">
         <f t="shared" si="8"/>
-        <v>153.77000000000032</v>
+        <v>95.495000000000118</v>
       </c>
       <c r="T24" s="26">
         <f t="shared" si="9"/>
@@ -2776,7 +2789,7 @@
       <c r="AE24" s="10"/>
       <c r="AF24" s="11"/>
     </row>
-    <row r="25" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E25" t="s">
         <v>10</v>
       </c>
@@ -2793,7 +2806,7 @@
       </c>
       <c r="I25" s="18">
         <f>AD25</f>
-        <v>71.489999999999995</v>
+        <v>67.650000000000006</v>
       </c>
       <c r="J25" s="14">
         <f>AC25</f>
@@ -2807,7 +2820,7 @@
       </c>
       <c r="M25" s="13">
         <f t="shared" ref="M25" si="13">I25*K25*$D$8*100*100</f>
-        <v>1251.0749999999998</v>
+        <v>1183.875</v>
       </c>
       <c r="N25" s="18">
         <f t="shared" ref="N25" si="14">J25*L25*$D$8*100*100</f>
@@ -2815,7 +2828,7 @@
       </c>
       <c r="O25" s="38">
         <f t="shared" si="5"/>
-        <v>0.75902407929180893</v>
+        <v>0.80210837292788495</v>
       </c>
       <c r="P25" s="40">
         <f t="shared" si="6"/>
@@ -2830,7 +2843,7 @@
       </c>
       <c r="S25" s="25">
         <f t="shared" si="8"/>
-        <v>301.47895000000005</v>
+        <v>234.27895000000024</v>
       </c>
       <c r="T25" s="26">
         <f t="shared" si="9"/>
@@ -2843,34 +2856,34 @@
         <v>53.12</v>
       </c>
       <c r="X25" s="31">
-        <v>61.86</v>
+        <v>58.02</v>
       </c>
       <c r="Y25" s="30">
         <v>50.03</v>
       </c>
       <c r="Z25" s="31">
-        <v>61.86</v>
+        <v>58.02</v>
       </c>
       <c r="AA25" s="30">
         <v>45</v>
       </c>
       <c r="AB25" s="31">
-        <v>60.38</v>
+        <v>57.05</v>
       </c>
       <c r="AC25" s="30">
         <v>48.88</v>
       </c>
       <c r="AD25" s="31">
-        <v>71.489999999999995</v>
+        <v>67.650000000000006</v>
       </c>
       <c r="AE25" s="30">
         <v>50.55</v>
       </c>
       <c r="AF25" s="31">
-        <v>94.19</v>
+        <v>84.59</v>
       </c>
     </row>
-    <row r="26" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E26" t="s">
         <v>10</v>
       </c>
@@ -2887,7 +2900,7 @@
       </c>
       <c r="I26" s="20">
         <f>AF25</f>
-        <v>94.19</v>
+        <v>84.59</v>
       </c>
       <c r="J26" s="16">
         <f>AE25</f>
@@ -2901,7 +2914,7 @@
       </c>
       <c r="M26" s="15">
         <f t="shared" ref="M26" si="15">I26*K26*$D$8*100*100</f>
-        <v>1648.3249999999998</v>
+        <v>1480.3250000000003</v>
       </c>
       <c r="N26" s="20">
         <f t="shared" ref="N26" si="16">J26*L26*$D$8*100*100</f>
@@ -2909,7 +2922,7 @@
       </c>
       <c r="O26" s="39">
         <f t="shared" si="5"/>
-        <v>0.62066767779412424</v>
+        <v>0.69110637866684654</v>
       </c>
       <c r="P26" s="41">
         <f t="shared" si="6"/>
@@ -2924,14 +2937,14 @@
       </c>
       <c r="S26" s="27">
         <f t="shared" si="8"/>
-        <v>625.26295000000005</v>
+        <v>457.2629500000005</v>
       </c>
       <c r="T26" s="28">
         <f t="shared" si="9"/>
         <v>38.48795000000041</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="G28" t="s">
         <v>11</v>
       </c>

</xml_diff>